<commit_message>
Got very close results, trying something else
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -2,22 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC5AF39-AE92-405B-8557-089A29A66209}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3DC07C-C8F4-4FBB-BE1C-1E309A88C9CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
   <si>
     <t>HK-2</t>
   </si>
@@ -155,75 +153,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet4"/>
-      <sheetName val="kpl"/>
-      <sheetName val="Sheet8"/>
-      <sheetName val="KMCT4"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="38">
-          <cell r="G38" t="str">
-            <v>HK-2</v>
-          </cell>
-          <cell r="H38" t="str">
-            <v>UMRC6</v>
-          </cell>
-          <cell r="I38" t="str">
-            <v>UOK262</v>
-          </cell>
-          <cell r="J38" t="str">
-            <v>UOK + DIDS</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="F39" t="str">
-            <v>KMCT4</v>
-          </cell>
-          <cell r="G39">
-            <v>0.15246154644866769</v>
-          </cell>
-          <cell r="H39">
-            <v>0.64294411858870992</v>
-          </cell>
-          <cell r="I39">
-            <v>1.3683853881971031</v>
-          </cell>
-          <cell r="J39">
-            <v>0.42186206704651613</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="G40">
-            <v>3.6118128467763112E-2</v>
-          </cell>
-          <cell r="H40">
-            <v>0.12580915640925344</v>
-          </cell>
-          <cell r="I40">
-            <v>0.77578226166599928</v>
-          </cell>
-          <cell r="J40">
-            <v>0.34549508550384522</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -523,10 +452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367D4110-0F05-4AA9-9660-0497C0778528}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J52" sqref="J52:M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,28 +466,28 @@
         <v>48.120613911731617</v>
       </c>
       <c r="B1">
-        <v>3.766371852901853E-3</v>
+        <v>3.4795161265732725E-3</v>
       </c>
       <c r="C1">
-        <v>0.12086913101524059</v>
+        <v>0.12115537047460399</v>
       </c>
       <c r="D1">
-        <v>28.28612704716037</v>
+        <v>28.286127101148843</v>
       </c>
       <c r="E1">
-        <v>2.6000863729608492E-14</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F1">
-        <v>0.25687767252350868</v>
+        <v>0.22199757443326015</v>
       </c>
       <c r="G1">
-        <v>36.700000000000003</v>
+        <v>37.450343333468659</v>
       </c>
       <c r="H1">
-        <v>0.17294782921976157</v>
+        <v>0.1193170263614496</v>
       </c>
       <c r="I1">
-        <v>0.17313318279239676</v>
+        <v>0.1411298456931295</v>
       </c>
       <c r="J1">
         <v>2.356211808499348</v>
@@ -569,22 +499,22 @@
         <v>254686091.39268142</v>
       </c>
       <c r="M1">
-        <v>0.99715195350250307</v>
+        <v>0.99715195462511363</v>
       </c>
       <c r="N1">
-        <v>0.99784243172281495</v>
+        <v>0.99785346972528499</v>
       </c>
       <c r="O1">
-        <v>0.99463045778084602</v>
+        <v>0.99488532535510454</v>
       </c>
       <c r="P1">
-        <v>7.6353436521167398E-2</v>
+        <v>7.6353436469702843E-2</v>
       </c>
       <c r="Q1">
-        <v>6.6242518908680145E-2</v>
+        <v>6.5139118584084318E-2</v>
       </c>
       <c r="R1">
-        <v>0.13556444167640569</v>
+        <v>0.13102591930261462</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -592,25 +522,25 @@
         <v>50.680396451715154</v>
       </c>
       <c r="B2">
-        <v>3.9270150205784546E-3</v>
+        <v>3.9270147990883662E-3</v>
       </c>
       <c r="C2">
-        <v>0.21794698560652839</v>
+        <v>0.21794698582814859</v>
       </c>
       <c r="D2">
         <v>9.9009938275001232</v>
       </c>
       <c r="E2">
-        <v>2.2800426908737547E-14</v>
+        <v>2.2205996670362198E-14</v>
       </c>
       <c r="F2">
-        <v>0.11894112148511023</v>
+        <v>0.11894110934795486</v>
       </c>
       <c r="G2">
-        <v>36.700000000000003</v>
+        <v>37.648702144402527</v>
       </c>
       <c r="H2">
-        <v>7.4859008109161324E-2</v>
+        <v>4.8297651990673832E-2</v>
       </c>
       <c r="I2">
         <v>2.2204460492503131E-14</v>
@@ -625,22 +555,22 @@
         <v>161047158.1115168</v>
       </c>
       <c r="M2">
-        <v>0.99709416769265757</v>
+        <v>0.99709416769265702</v>
       </c>
       <c r="N2">
-        <v>0.98619132325723524</v>
+        <v>0.98619132265690701</v>
       </c>
       <c r="O2">
-        <v>0.99689204471539772</v>
+        <v>0.99689204548862798</v>
       </c>
       <c r="P2">
-        <v>7.6844094339646438E-2</v>
+        <v>7.6844094339646424E-2</v>
       </c>
       <c r="Q2">
-        <v>0.16808999018197815</v>
+        <v>0.16808999389977516</v>
       </c>
       <c r="R2">
-        <v>7.8981915870372454E-2</v>
+        <v>7.8981907325062134E-2</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -648,28 +578,28 @@
         <v>49.102731389712162</v>
       </c>
       <c r="B3">
-        <v>5.18692778497961E-3</v>
+        <v>3.5726191661664243E-3</v>
       </c>
       <c r="C3">
-        <v>0.2299887797931762</v>
+        <v>0.23160370685789064</v>
       </c>
       <c r="D3">
-        <v>24.26160006575941</v>
+        <v>23.523827043276164</v>
       </c>
       <c r="E3">
-        <v>4.4387531143817071E-14</v>
+        <v>2.2219642502235133E-14</v>
       </c>
       <c r="F3">
-        <v>0.18363991970032575</v>
+        <v>0.10008818132332642</v>
       </c>
       <c r="G3">
-        <v>36.700000000000003</v>
+        <v>37.632295288329871</v>
       </c>
       <c r="H3">
-        <v>0.20825290332918217</v>
+        <v>6.0138209620568157E-2</v>
       </c>
       <c r="I3">
-        <v>1.0754343931403764E-7</v>
+        <v>2.2230487406924265E-14</v>
       </c>
       <c r="J3">
         <v>2.8545008818278075</v>
@@ -681,22 +611,22 @@
         <v>491427690.54543257</v>
       </c>
       <c r="M3">
-        <v>0.99564380041429623</v>
+        <v>0.99564380003670339</v>
       </c>
       <c r="N3">
-        <v>0.99558186714849217</v>
+        <v>0.99195335998266976</v>
       </c>
       <c r="O3">
-        <v>0.97704050815832943</v>
+        <v>0.9975015329873631</v>
       </c>
       <c r="P3">
-        <v>9.5112350342765176E-2</v>
+        <v>9.5112350349509781E-2</v>
       </c>
       <c r="Q3">
-        <v>9.4451350748225624E-2</v>
+        <v>0.12686716616817512</v>
       </c>
       <c r="R3">
-        <v>0.22768544871195529</v>
+        <v>8.6621753913290897E-2</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -704,28 +634,28 @@
         <v>50.012571778454578</v>
       </c>
       <c r="B4">
-        <v>1.1317987599567918E-2</v>
+        <v>8.2261049334318315E-3</v>
       </c>
       <c r="C4">
-        <v>4.733752837913132E-3</v>
+        <v>7.8238786162331871E-3</v>
       </c>
       <c r="D4">
-        <v>24.127215671181709</v>
+        <v>24.126393645454886</v>
       </c>
       <c r="E4">
-        <v>2.0968412510602168E-9</v>
+        <v>8.4517983628408446E-7</v>
       </c>
       <c r="F4">
-        <v>0.51068369586521845</v>
+        <v>0.38417933083549277</v>
       </c>
       <c r="G4">
-        <v>36.700000000000003</v>
+        <v>35.700042294070279</v>
       </c>
       <c r="H4">
-        <v>0.51038435130899318</v>
+        <v>0.30888130275024206</v>
       </c>
       <c r="I4">
-        <v>4.1495593605238217E-14</v>
+        <v>4.1254209297634721E-14</v>
       </c>
       <c r="J4">
         <v>5.740537779224173</v>
@@ -737,22 +667,22 @@
         <v>142097848.58194768</v>
       </c>
       <c r="M4">
-        <v>0.99706205539937709</v>
+        <v>0.99706208406329411</v>
       </c>
       <c r="N4">
-        <v>0.95782389925554146</v>
+        <v>0.95451182918462252</v>
       </c>
       <c r="O4">
-        <v>0.97649329161720799</v>
+        <v>0.96755342148890255</v>
       </c>
       <c r="P4">
-        <v>7.8465814862986982E-2</v>
+        <v>7.8465803659368477E-2</v>
       </c>
       <c r="Q4">
-        <v>0.30237146456736597</v>
+        <v>0.29835113413949227</v>
       </c>
       <c r="R4">
-        <v>0.21852395338919081</v>
+        <v>0.25391303933089066</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -760,28 +690,28 @@
         <v>49.41571153061205</v>
       </c>
       <c r="B5">
-        <v>5.0584649382119408E-2</v>
+        <v>1.7952384844695909E-2</v>
       </c>
       <c r="C5">
-        <v>0.29250656648100509</v>
+        <v>0.32513897643519724</v>
       </c>
       <c r="D5">
-        <v>10.883479756748507</v>
+        <v>10.79063676008248</v>
       </c>
       <c r="E5">
-        <v>4.4408902883031692E-14</v>
+        <v>3.37910782375764E-14</v>
       </c>
       <c r="F5">
-        <v>1.9577181908346022</v>
+        <v>0.77012992110925338</v>
       </c>
       <c r="G5">
-        <v>36.700000000000003</v>
+        <v>37.372364258487238</v>
       </c>
       <c r="H5">
-        <v>1.8456110119580971</v>
+        <v>0.67099227523245808</v>
       </c>
       <c r="I5">
-        <v>3.3948376166350218E-8</v>
+        <v>4.1482880168662724E-14</v>
       </c>
       <c r="J5">
         <v>3.2019451544874276</v>
@@ -793,22 +723,22 @@
         <v>629017289.17440271</v>
       </c>
       <c r="M5">
-        <v>0.99609224848712852</v>
+        <v>0.99609224845038047</v>
       </c>
       <c r="N5">
-        <v>0.98327304120965686</v>
+        <v>0.98228022729653697</v>
       </c>
       <c r="O5">
-        <v>0.99161989441105292</v>
+        <v>0.99321581530579128</v>
       </c>
       <c r="P5">
-        <v>9.1131006251183325E-2</v>
+        <v>9.1131006252957447E-2</v>
       </c>
       <c r="Q5">
-        <v>0.18282770249212313</v>
+        <v>0.18801244877525125</v>
       </c>
       <c r="R5">
-        <v>0.12961365161034083</v>
+        <v>0.11728586191248075</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -816,28 +746,28 @@
         <v>49.428561200603092</v>
       </c>
       <c r="B6">
-        <v>1.2726416434731868E-2</v>
+        <v>1.2730246353966567E-2</v>
       </c>
       <c r="C6">
-        <v>1.7735025133817662E-6</v>
+        <v>1.0000022208952447E-8</v>
       </c>
       <c r="D6">
-        <v>24.198790583220934</v>
+        <v>24.295808480577492</v>
       </c>
       <c r="E6">
-        <v>6.4328712500142868E-5</v>
+        <v>2.2215914010445092E-14</v>
       </c>
       <c r="F6">
-        <v>0.40754068309921787</v>
+        <v>0.40192353025805466</v>
       </c>
       <c r="G6">
-        <v>36.700000000000003</v>
+        <v>36.165937552207858</v>
       </c>
       <c r="H6">
-        <v>0.22314952545464181</v>
+        <v>0.19368398855284627</v>
       </c>
       <c r="I6">
-        <v>3.3509619079525097E-4</v>
+        <v>2.2237737766946569E-14</v>
       </c>
       <c r="J6">
         <v>4.8009905427717481</v>
@@ -849,22 +779,22 @@
         <v>149956135.49829885</v>
       </c>
       <c r="M6">
-        <v>0.99720080144229406</v>
+        <v>0.99720075071810876</v>
       </c>
       <c r="N6">
-        <v>0.98951085526313376</v>
+        <v>0.98945232763408242</v>
       </c>
       <c r="O6">
-        <v>0.99613231467383812</v>
+        <v>0.99609594278900127</v>
       </c>
       <c r="P6">
-        <v>7.5644746580094305E-2</v>
+        <v>7.5644718612386044E-2</v>
       </c>
       <c r="Q6">
-        <v>0.15504155278892673</v>
+        <v>0.1539517645319253</v>
       </c>
       <c r="R6">
-        <v>0.10850460484326056</v>
+        <v>0.10849575202156349</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -872,28 +802,28 @@
         <v>49.134693742595658</v>
       </c>
       <c r="B7">
-        <v>1.2298622689444138E-2</v>
+        <v>1.1336378651585302E-2</v>
       </c>
       <c r="C7">
-        <v>1.5611099196749542E-2</v>
+        <v>1.6568061839038396E-2</v>
       </c>
       <c r="D7">
-        <v>22.496247993789488</v>
+        <v>21.79919917966312</v>
       </c>
       <c r="E7">
-        <v>1.2257795631052319E-4</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F7">
-        <v>9.2203674952512596E-2</v>
+        <v>7.6265635306323493E-2</v>
       </c>
       <c r="G7">
-        <v>36.700000000000003</v>
+        <v>36.153317535502289</v>
       </c>
       <c r="H7">
-        <v>0.16525155478360823</v>
+        <v>9.8533251240757375E-2</v>
       </c>
       <c r="I7">
-        <v>9.4776284862304136E-9</v>
+        <v>2.2204979238374094E-14</v>
       </c>
       <c r="J7">
         <v>1.952898836424503</v>
@@ -905,22 +835,22 @@
         <v>132744891.08503906</v>
       </c>
       <c r="M7">
-        <v>0.99900215809722059</v>
+        <v>0.99900216768483463</v>
       </c>
       <c r="N7">
-        <v>0.99841094552876042</v>
+        <v>0.99812720704547231</v>
       </c>
       <c r="O7">
-        <v>0.99344726515956139</v>
+        <v>0.9965996225501188</v>
       </c>
       <c r="P7">
-        <v>4.444848003844535E-2</v>
+        <v>4.4448064950350752E-2</v>
       </c>
       <c r="Q7">
-        <v>6.0065850458378575E-2</v>
+        <v>6.3844926603594698E-2</v>
       </c>
       <c r="R7">
-        <v>0.12364646515234076</v>
+        <v>9.123185443573037E-2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -928,28 +858,28 @@
         <v>48.970224341450667</v>
       </c>
       <c r="B8">
-        <v>2.2011934502965087E-2</v>
+        <v>2.8455085625926618E-2</v>
       </c>
       <c r="C8">
-        <v>0.20827938782863858</v>
+        <v>0.19463910134944526</v>
       </c>
       <c r="D8">
-        <v>15.382937618173871</v>
+        <v>15.382937678032819</v>
       </c>
       <c r="E8">
-        <v>8.9208069875109847E-2</v>
+        <v>2.4898037270932147E-3</v>
       </c>
       <c r="F8">
-        <v>7.6601702963920812E-2</v>
+        <v>0.23965150048870829</v>
       </c>
       <c r="G8">
-        <v>36.700000000000003</v>
+        <v>36.927912625888425</v>
       </c>
       <c r="H8">
-        <v>0.15128080732450089</v>
+        <v>0.57170256654956031</v>
       </c>
       <c r="I8">
-        <v>2.2204567639732937E-14</v>
+        <v>9.941866654942422E-7</v>
       </c>
       <c r="J8">
         <v>2.4430206679346318</v>
@@ -961,22 +891,22 @@
         <v>457955160.74923623</v>
       </c>
       <c r="M8">
-        <v>0.99838221935492832</v>
+        <v>0.99837928576034285</v>
       </c>
       <c r="N8">
-        <v>0.99734885461055078</v>
+        <v>0.99840550035107978</v>
       </c>
       <c r="O8">
-        <v>0.99710079889684633</v>
+        <v>0.97812854760325485</v>
       </c>
       <c r="P8">
-        <v>5.7537209680454934E-2</v>
+        <v>5.751194069035951E-2</v>
       </c>
       <c r="Q8">
-        <v>7.238187956708346E-2</v>
+        <v>5.6148136508280842E-2</v>
       </c>
       <c r="R8">
-        <v>7.770256209451927E-2</v>
+        <v>0.21109361441809982</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -984,28 +914,28 @@
         <v>50.361069671134324</v>
       </c>
       <c r="B9">
-        <v>2.4353050512641725E-2</v>
+        <v>6.9060525830266173E-2</v>
       </c>
       <c r="C9">
-        <v>0.30271861804172473</v>
+        <v>0.25801108459089117</v>
       </c>
       <c r="D9">
-        <v>13.350160601214489</v>
+        <v>13.471631554455945</v>
       </c>
       <c r="E9">
-        <v>2.2204460492503131E-14</v>
+        <v>2.9250814687839763E-14</v>
       </c>
       <c r="F9">
-        <v>1.2785105518916953</v>
+        <v>3.2253352307515293</v>
       </c>
       <c r="G9">
-        <v>36.700000000000003</v>
+        <v>35.700000003988414</v>
       </c>
       <c r="H9">
-        <v>3.9999999999999778</v>
+        <v>9.750654659613712</v>
       </c>
       <c r="I9">
-        <v>2.2210375778476466E-14</v>
+        <v>8.9507003447047568E-9</v>
       </c>
       <c r="J9">
         <v>4.3363113643580764</v>
@@ -1017,22 +947,22 @@
         <v>1205583684.8478703</v>
       </c>
       <c r="M9">
-        <v>0.99455792352173955</v>
+        <v>0.99455792352757189</v>
       </c>
       <c r="N9">
-        <v>0.95852362177719175</v>
+        <v>0.95888050748856335</v>
       </c>
       <c r="O9">
-        <v>0.98146081451281919</v>
+        <v>0.98176164041495118</v>
       </c>
       <c r="P9">
-        <v>0.10398649260519804</v>
+        <v>0.10398649260370561</v>
       </c>
       <c r="Q9">
-        <v>0.29868722901286959</v>
+        <v>0.29760772423271709</v>
       </c>
       <c r="R9">
-        <v>0.20042575722777428</v>
+        <v>0.19874222923660653</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1040,28 +970,28 @@
         <v>50.999999997994593</v>
       </c>
       <c r="B10">
-        <v>9.1077088721184113E-3</v>
+        <v>1.2323139929023586E-2</v>
       </c>
       <c r="C10">
-        <v>1.8804174558085654E-2</v>
+        <v>1.5598276110641449E-2</v>
       </c>
       <c r="D10">
-        <v>16.049210793904102</v>
+        <v>16.049210786922742</v>
       </c>
       <c r="E10">
-        <v>3.358470715247496E-14</v>
+        <v>1.0730907695642397E-3</v>
       </c>
       <c r="F10">
-        <v>0.91828502012450097</v>
+        <v>1.2599420336012488</v>
       </c>
       <c r="G10">
-        <v>36.700000000000003</v>
+        <v>36.583994487306306</v>
       </c>
       <c r="H10">
-        <v>1.0682402232376766</v>
+        <v>1.4553538898315348</v>
       </c>
       <c r="I10">
-        <v>3.3170459724499869E-14</v>
+        <v>4.0807233768722193E-14</v>
       </c>
       <c r="J10">
         <v>3.6193816110419976</v>
@@ -1073,22 +1003,22 @@
         <v>83209857.156356871</v>
       </c>
       <c r="M10">
-        <v>0.99668268126311965</v>
+        <v>0.99668267063118265</v>
       </c>
       <c r="N10">
-        <v>0.98913141317433029</v>
+        <v>0.98967172348163557</v>
       </c>
       <c r="O10">
-        <v>0.99192549164409527</v>
+        <v>0.99072332294345355</v>
       </c>
       <c r="P10">
-        <v>8.1022431703491687E-2</v>
+        <v>8.1022592759074114E-2</v>
       </c>
       <c r="Q10">
-        <v>0.14931894650639582</v>
+        <v>0.1457665294218416</v>
       </c>
       <c r="R10">
-        <v>0.12670129057303417</v>
+        <v>0.13578312841773169</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1096,28 +1026,28 @@
         <v>50.99993380168803</v>
       </c>
       <c r="B11">
-        <v>1.717293583587242E-2</v>
+        <v>1.601888853618769E-2</v>
       </c>
       <c r="C11">
-        <v>0.1630178155852034</v>
+        <v>0.1641584912521373</v>
       </c>
       <c r="D11">
-        <v>22.716652885752577</v>
+        <v>22.08294010390086</v>
       </c>
       <c r="E11">
-        <v>1.8535656710339093E-4</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F11">
-        <v>0.12763432519159332</v>
+        <v>0.11219420894660005</v>
       </c>
       <c r="G11">
-        <v>36.700000000000003</v>
+        <v>37.398012035506362</v>
       </c>
       <c r="H11">
-        <v>0.25768730528318334</v>
+        <v>0.19245141659030984</v>
       </c>
       <c r="I11">
-        <v>5.617302640694877E-9</v>
+        <v>2.2206781588809361E-14</v>
       </c>
       <c r="J11">
         <v>2.8612100103634148</v>
@@ -1129,22 +1059,22 @@
         <v>44059879.020455331</v>
       </c>
       <c r="M11">
-        <v>0.99213819741193987</v>
+        <v>0.99213822043396482</v>
       </c>
       <c r="N11">
-        <v>0.9942669422383259</v>
+        <v>0.99410838184506134</v>
       </c>
       <c r="O11">
-        <v>0.99221007666910066</v>
+        <v>0.99319548348425291</v>
       </c>
       <c r="P11">
-        <v>0.12446947614223271</v>
+        <v>0.12446931357457527</v>
       </c>
       <c r="Q11">
-        <v>0.1162341406818679</v>
+        <v>0.11716632920010855</v>
       </c>
       <c r="R11">
-        <v>0.15430822566210037</v>
+        <v>0.14608669072309458</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1152,28 +1082,28 @@
         <v>50.112410423624041</v>
       </c>
       <c r="B12">
-        <v>7.999999999996267E-2</v>
+        <v>7.9999999969555299E-2</v>
       </c>
       <c r="C12">
-        <v>2.025479341410787</v>
+        <v>2.025498154431006</v>
       </c>
       <c r="D12">
-        <v>26.71596083305791</v>
+        <v>26.715960833056617</v>
       </c>
       <c r="E12">
-        <v>3.9968399461233248E-14</v>
+        <v>4.813190262085224E-11</v>
       </c>
       <c r="F12">
-        <v>0.17802721935542151</v>
+        <v>0.17802513032889813</v>
       </c>
       <c r="G12">
-        <v>36.700000000000003</v>
+        <v>37.653887362839399</v>
       </c>
       <c r="H12">
-        <v>0.40025662643556598</v>
+        <v>0.37369127504783234</v>
       </c>
       <c r="I12">
-        <v>4.0626459604112994E-14</v>
+        <v>4.2438187820793242E-14</v>
       </c>
       <c r="J12">
         <v>5.3408895358905601</v>
@@ -1185,22 +1115,22 @@
         <v>1300249383.1199305</v>
       </c>
       <c r="M12">
-        <v>0.97974716331867562</v>
+        <v>0.97974716357598268</v>
       </c>
       <c r="N12">
-        <v>0.92111195828092951</v>
+        <v>0.92111167361335022</v>
       </c>
       <c r="O12">
-        <v>0.96654902334635584</v>
+        <v>0.96654862729160018</v>
       </c>
       <c r="P12">
-        <v>0.20055742933618792</v>
+        <v>0.20055742706207924</v>
       </c>
       <c r="Q12">
-        <v>0.38892937991952131</v>
+        <v>0.38892998015242602</v>
       </c>
       <c r="R12">
-        <v>0.25541822032929429</v>
+        <v>0.25541943931821498</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1208,28 +1138,28 @@
         <v>50.170242659167336</v>
       </c>
       <c r="B13">
-        <v>9.626456283729868E-3</v>
+        <v>8.6403546782031753E-3</v>
       </c>
       <c r="C13">
-        <v>6.9009974449543779E-2</v>
+        <v>6.9996504707704105E-2</v>
       </c>
       <c r="D13">
-        <v>23.866913434530208</v>
+        <v>24.289359659065365</v>
       </c>
       <c r="E13">
-        <v>2.2204460492503131E-14</v>
+        <v>5.5774294888870558E-10</v>
       </c>
       <c r="F13">
-        <v>0.17272069181479041</v>
+        <v>0.14710121465685502</v>
       </c>
       <c r="G13">
-        <v>36.700000000000003</v>
+        <v>36.223814614921984</v>
       </c>
       <c r="H13">
-        <v>0.61595767628621578</v>
+        <v>0.48172107020411004</v>
       </c>
       <c r="I13">
-        <v>2.220462387609877E-14</v>
+        <v>3.1310055328609909E-14</v>
       </c>
       <c r="J13">
         <v>4.079138265678818</v>
@@ -1241,22 +1171,22 @@
         <v>566450101.24093688</v>
       </c>
       <c r="M13">
-        <v>0.99898533054488625</v>
+        <v>0.99898533074451068</v>
       </c>
       <c r="N13">
-        <v>0.99766732262067337</v>
+        <v>0.99701139548014506</v>
       </c>
       <c r="O13">
-        <v>0.942208645181007</v>
+        <v>0.949541110127199</v>
       </c>
       <c r="P13">
-        <v>4.4815903396743711E-2</v>
+        <v>4.4815903611969979E-2</v>
       </c>
       <c r="Q13">
-        <v>7.4461511200816233E-2</v>
+        <v>8.2400008207427697E-2</v>
       </c>
       <c r="R13">
-        <v>0.34675211622933355</v>
+        <v>0.32512088803992523</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1264,28 +1194,28 @@
         <v>50.757253125081057</v>
       </c>
       <c r="B14">
-        <v>4.8531909184495198E-3</v>
+        <v>4.8323620306448935E-3</v>
       </c>
       <c r="C14">
-        <v>5.4349222096339821E-3</v>
+        <v>5.4563962150907331E-3</v>
       </c>
       <c r="D14">
-        <v>24.502054117453266</v>
+        <v>24.502054124559894</v>
       </c>
       <c r="E14">
-        <v>2.2204615595947165E-14</v>
+        <v>1.7651220104339856E-5</v>
       </c>
       <c r="F14">
-        <v>3.196788972578541E-2</v>
+        <v>3.1617351973594027E-2</v>
       </c>
       <c r="G14">
-        <v>36.700000000000003</v>
+        <v>36.697236947356437</v>
       </c>
       <c r="H14">
-        <v>7.7203191407488742E-2</v>
+        <v>4.7124138988605048E-2</v>
       </c>
       <c r="I14">
-        <v>2.2204881513572283E-14</v>
+        <v>1.6211893547391038E-5</v>
       </c>
       <c r="J14">
         <v>4.5658015908569123</v>
@@ -1297,22 +1227,22 @@
         <v>350999697.1980691</v>
       </c>
       <c r="M14">
-        <v>0.9920818371300455</v>
+        <v>0.99208181807768536</v>
       </c>
       <c r="N14">
-        <v>0.99509847608947144</v>
+        <v>0.99508377256621872</v>
       </c>
       <c r="O14">
-        <v>0.9922351333664543</v>
+        <v>0.99253225813286505</v>
       </c>
       <c r="P14">
-        <v>0.12573147808382565</v>
+        <v>0.12573170714751689</v>
       </c>
       <c r="Q14">
-        <v>0.1022233940204005</v>
+        <v>0.10237015179103715</v>
       </c>
       <c r="R14">
-        <v>0.12736064836786898</v>
+        <v>0.12637696756741412</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1320,28 +1250,28 @@
         <v>50.897187024056102</v>
       </c>
       <c r="B15">
-        <v>9.6278714299081834E-3</v>
+        <v>1.1560450572118007E-2</v>
       </c>
       <c r="C15">
-        <v>8.9047001271310683E-2</v>
+        <v>8.4848356183085338E-2</v>
       </c>
       <c r="D15">
-        <v>11.269070922303309</v>
+        <v>11.269071995275183</v>
       </c>
       <c r="E15">
-        <v>5.6390814252163898E-2</v>
+        <v>2.407360763413255E-14</v>
       </c>
       <c r="F15">
-        <v>4.9463077002217568E-2</v>
+        <v>0.15210747569666191</v>
       </c>
       <c r="G15">
-        <v>36.700000000000003</v>
+        <v>37.577766937274333</v>
       </c>
       <c r="H15">
-        <v>4.4281078239474005E-2</v>
+        <v>0.22793467277447976</v>
       </c>
       <c r="I15">
-        <v>2.2204475114886974E-14</v>
+        <v>3.8305931461935391E-14</v>
       </c>
       <c r="J15">
         <v>6.1031742274447058</v>
@@ -1353,22 +1283,22 @@
         <v>621934179.43162954</v>
       </c>
       <c r="M15">
-        <v>0.99881950193018176</v>
+        <v>0.99882163160938198</v>
       </c>
       <c r="N15">
-        <v>0.99064358009197151</v>
+        <v>0.99270388667667397</v>
       </c>
       <c r="O15">
-        <v>0.99551991946483143</v>
+        <v>0.96037915720805644</v>
       </c>
       <c r="P15">
-        <v>4.8333595553137078E-2</v>
+        <v>4.8286264033468369E-2</v>
       </c>
       <c r="Q15">
-        <v>0.13658325063364676</v>
+        <v>0.12081206714507217</v>
       </c>
       <c r="R15">
-        <v>9.4634400610573904E-2</v>
+        <v>0.28282810134363656</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1376,28 +1306,28 @@
         <v>49.372704065629407</v>
       </c>
       <c r="B16">
-        <v>2.1402952667122423E-2</v>
+        <v>4.4712314332643145E-2</v>
       </c>
       <c r="C16">
-        <v>0.36277645600389541</v>
+        <v>0.33865466146936779</v>
       </c>
       <c r="D16">
-        <v>9.9724964153968099</v>
+        <v>9.9724964073016142</v>
       </c>
       <c r="E16">
-        <v>3.9391687055648723E-2</v>
+        <v>2.2204460492503131E-14</v>
       </c>
       <c r="F16">
-        <v>1.0273341409311201</v>
+        <v>1.8828390630124936</v>
       </c>
       <c r="G16">
-        <v>36.700000000000003</v>
+        <v>35.700000000028353</v>
       </c>
       <c r="H16">
-        <v>3.9999999999999631</v>
+        <v>9.9999999999999787</v>
       </c>
       <c r="I16">
-        <v>0.22750166907634406</v>
+        <v>4.8819468832966442E-10</v>
       </c>
       <c r="J16">
         <v>2.8975994027540488</v>
@@ -1409,22 +1339,22 @@
         <v>818269300.73777747</v>
       </c>
       <c r="M16">
-        <v>0.99463958640116923</v>
+        <v>0.99463967383988361</v>
       </c>
       <c r="N16">
-        <v>0.98527885621225764</v>
+        <v>0.985550803068721</v>
       </c>
       <c r="O16">
-        <v>0.9700846846807285</v>
+        <v>0.96924532881281233</v>
       </c>
       <c r="P16">
-        <v>0.10311984323775644</v>
+        <v>0.10311916123851592</v>
       </c>
       <c r="Q16">
-        <v>0.20055166698685833</v>
+        <v>0.19758020614782132</v>
       </c>
       <c r="R16">
-        <v>0.46293537294677184</v>
+        <v>0.24695341960909117</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -1733,26 +1663,26 @@
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>STDEV(B5:B16)/SQRT(12)</f>
-        <v>6.2455093474297514E-3</v>
+        <v>7.1901822400319594E-3</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23">
         <f>AVERAGE(B$1:B$3)</f>
-        <v>4.293438219486639E-3</v>
+        <v>3.6597166972760207E-3</v>
       </c>
       <c r="D23">
         <f>AVERAGE(B$4:B$6)</f>
-        <v>2.4876351138806398E-2</v>
+        <v>1.2969578710698102E-2</v>
       </c>
       <c r="E23">
         <f>AVERAGE(B$9:B$11)</f>
-        <v>1.6877898406877517E-2</v>
+        <v>3.2467518098492486E-2</v>
       </c>
       <c r="F23">
         <f>AVERAGE(B$13:B$16)</f>
-        <v>1.1377617824802498E-2</v>
+        <v>1.7436370403402304E-2</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
@@ -1794,19 +1724,19 @@
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C24">
         <f>STDEV(B$1:B$3)/SQRT(COUNT(B$1:B$3))</f>
-        <v>4.4914521021005609E-4</v>
+        <v>1.3632467423976377E-4</v>
       </c>
       <c r="D24">
         <f>STDEV(B$4:B$6)/SQRT(COUNT(B$4:B$6))</f>
-        <v>1.2860577577378065E-2</v>
+        <v>2.8102841025300172E-3</v>
       </c>
       <c r="E24">
         <f>STDEV(B$9:B$11)/SQRT(COUNT(B$9:B$11))</f>
-        <v>4.4034227500680118E-3</v>
+        <v>1.8327582133541017E-2</v>
       </c>
       <c r="F24">
         <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
-        <v>3.5261365111874943E-3</v>
+        <v>9.1957167148318739E-3</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
@@ -1939,19 +1869,19 @@
       </c>
       <c r="D27">
         <f>AVERAGE(C$1:C$3)</f>
-        <v>0.18960163213831505</v>
+        <v>0.19023535438688108</v>
       </c>
       <c r="E27">
         <f>AVERAGE(C$4:C$6)</f>
-        <v>9.9080697607143872E-2</v>
+        <v>0.11098762168381754</v>
       </c>
       <c r="F27">
         <f>AVERAGE(C$9:C$11)</f>
-        <v>0.16151353606167126</v>
+        <v>0.14592261731789</v>
       </c>
       <c r="G27">
         <f>AVERAGE(C$13:C$16)</f>
-        <v>0.13156708848359597</v>
+        <v>0.12473897964381199</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
@@ -1993,19 +1923,19 @@
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D28">
         <f>STDEV(C$1:C$3)/SQRT(COUNT(C$1:C$3))</f>
-        <v>3.4541611305706231E-2</v>
+        <v>3.4764251947037965E-2</v>
       </c>
       <c r="E28">
         <f>STDEV(C$4:C$6)/SQRT(COUNT(C$4:C$6))</f>
-        <v>9.6722580902485894E-2</v>
+        <v>0.10709949468666879</v>
       </c>
       <c r="F28">
         <f>STDEV(C$9:C$11)/SQRT(COUNT(C$9:C$11))</f>
-        <v>8.1962491314258729E-2</v>
+        <v>7.0570066251987876E-2</v>
       </c>
       <c r="G28">
         <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
-        <v>7.9103542551787268E-2</v>
+        <v>7.3357716046404037E-2</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
@@ -2135,26 +2065,26 @@
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>STDEV(D5:D16)/SQRT(12)</f>
-        <v>1.7917879182695247</v>
+        <v>1.783009832631351</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31">
         <f>AVERAGE(D$1:D$3)</f>
-        <v>20.816240313473301</v>
+        <v>20.57031599064171</v>
       </c>
       <c r="F31">
         <f>AVERAGE(D$4:D$6)</f>
-        <v>19.736495337050382</v>
+        <v>19.737612962038288</v>
       </c>
       <c r="G31">
         <f>AVERAGE(D$9:D$11)</f>
-        <v>17.372008093623723</v>
+        <v>17.201260815093182</v>
       </c>
       <c r="H31">
         <f>AVERAGE(D$13:D$16)</f>
-        <v>17.402633722420898</v>
+        <v>17.508245546550516</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
@@ -2196,23 +2126,23 @@
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>MIN(D5:D14)</f>
-        <v>10.883479756748507</v>
+        <v>10.79063676008248</v>
       </c>
       <c r="E32">
         <f>STDEV(D$1:D$3)/SQRT(COUNT(D$1:D$3))</f>
-        <v>5.5799091612429308</v>
+        <v>5.508953379907469</v>
       </c>
       <c r="F32">
         <f>STDEV(D$4:D$6)/SQRT(COUNT(D$4:D$6))</f>
-        <v>4.4265560123271639</v>
+        <v>4.47375542154324</v>
       </c>
       <c r="G32">
         <f>STDEV(D$9:D$11)/SQRT(COUNT(D$9:D$11))</f>
-        <v>2.7835911428217388</v>
+        <v>2.5517362183417642</v>
       </c>
       <c r="H32">
         <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
-        <v>3.9265783998922781</v>
+        <v>3.9855119780421515</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
@@ -2254,7 +2184,7 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>MAX(G5:G14)</f>
-        <v>36.700000000000003</v>
+        <v>37.653887362839399</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2277,37 +2207,37 @@
       </c>
       <c r="F35">
         <f>AVERAGE(E$1:E$3)</f>
-        <v>3.1062940594054371E-14</v>
+        <v>2.2210033221700154E-14</v>
       </c>
       <c r="G35">
         <f>AVERAGE(E$4:E$6)</f>
-        <v>2.1443603128600944E-5</v>
+        <v>2.8172663076369224E-7</v>
       </c>
       <c r="H35">
         <f>AVERAGE(E$9:E$11)</f>
-        <v>6.1785522386393371E-5</v>
+        <v>3.5769692320523168E-4</v>
       </c>
       <c r="I35">
         <f>AVERAGE(E$13:E$16)</f>
-        <v>2.3945625326964259E-2</v>
+        <v>4.4129444733917032E-6</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F36">
         <f>STDEV(E$1:E$3)/SQRT(COUNT(E$1:E$3))</f>
-        <v>6.7260497061850448E-15</v>
+        <v>4.8250618270174104E-18</v>
       </c>
       <c r="G36">
         <f>STDEV(E$4:E$6)/SQRT(COUNT(E$4:E$6))</f>
-        <v>2.144255469431425E-5</v>
+        <v>2.8172660276019622E-7</v>
       </c>
       <c r="H36">
         <f>STDEV(E$9:E$11)/SQRT(COUNT(E$9:E$11))</f>
-        <v>6.1785522358498801E-5</v>
+        <v>3.5769692317950405E-4</v>
       </c>
       <c r="I36">
         <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
-        <v>1.4253821276868195E-2</v>
+        <v>4.4127585456074152E-6</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2327,44 +2257,44 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E39">
         <f>STDEV(F5:F16)/SQRT(12)</f>
-        <v>0.18051319836815735</v>
+        <v>0.28143020453412104</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
       </c>
       <c r="G39">
         <f>AVERAGE(F$1:F$3)</f>
-        <v>0.18648623790298155</v>
+        <v>0.14700895503484715</v>
       </c>
       <c r="H39">
         <f>AVERAGE(F$4:F$6)</f>
-        <v>0.95864752326634617</v>
+        <v>0.51874426073426694</v>
       </c>
       <c r="I39">
         <f>AVERAGE(F$9:F$11)</f>
-        <v>0.77480996573592975</v>
+        <v>1.5324904910997927</v>
       </c>
       <c r="J39">
         <f>AVERAGE(F$13:F$16)</f>
-        <v>0.32037144986847838</v>
+        <v>0.55341627633490109</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G40">
         <f>STDEV(F$1:F$3)/SQRT(COUNT(F$1:F$3))</f>
-        <v>3.9844276768335893E-2</v>
+        <v>3.7887236211488991E-2</v>
       </c>
       <c r="H40">
         <f>STDEV(F$4:F$6)/SQRT(COUNT(F$4:F$6))</f>
-        <v>0.50042191177947459</v>
+        <v>0.12579716058654763</v>
       </c>
       <c r="I40">
         <f>STDEV(F$9:F$11)/SQRT(COUNT(F$9:F$11))</f>
-        <v>0.33988617737889792</v>
+        <v>0.9089597995648262</v>
       </c>
       <c r="J40">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
-        <v>0.23772619980774551</v>
+        <v>0.44401386483779698</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2387,37 +2317,37 @@
       </c>
       <c r="H43">
         <f>AVERAGE(G$1:G$3)</f>
-        <v>36.700000000000003</v>
+        <v>37.577113588733688</v>
       </c>
       <c r="I43">
         <f>AVERAGE(G$4:G$6)</f>
-        <v>36.700000000000003</v>
+        <v>36.412781368255118</v>
       </c>
       <c r="J43">
         <f>AVERAGE(G$9:G$11)</f>
-        <v>36.700000000000003</v>
+        <v>36.560668842267027</v>
       </c>
       <c r="K43">
         <f>AVERAGE(G$13:G$16)</f>
-        <v>36.700000000000003</v>
+        <v>36.549704624895277</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H44">
         <f>STDEV(G$1:G$3)/SQRT(COUNT(G$1:G$3))</f>
-        <v>0</v>
+        <v>6.3561831960480958E-2</v>
       </c>
       <c r="I44">
         <f>STDEV(G$4:G$6)/SQRT(COUNT(G$4:G$6))</f>
-        <v>0</v>
+        <v>0.49828508918370279</v>
       </c>
       <c r="J44">
         <f>STDEV(G$9:G$11)/SQRT(COUNT(G$9:G$11))</f>
-        <v>0</v>
+        <v>0.49031258025953905</v>
       </c>
       <c r="K44">
         <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
-        <v>0</v>
+        <v>0.39863100653210481</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2440,37 +2370,37 @@
       </c>
       <c r="I47">
         <f>AVERAGE(H$1:H$3)</f>
-        <v>0.1520199135527017</v>
+        <v>7.5917629324230532E-2</v>
       </c>
       <c r="J47">
         <f>AVERAGE(H$4:H$6)</f>
-        <v>0.85971496290724403</v>
+        <v>0.39118585551184881</v>
       </c>
       <c r="K47">
         <f>AVERAGE(H$9:H$11)</f>
-        <v>1.7753091761736126</v>
+        <v>3.7994866553451856</v>
       </c>
       <c r="L47">
         <f>AVERAGE(H$13:H$16)</f>
-        <v>1.1843604864832855</v>
+        <v>2.6891949704917932</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I48">
         <f>STDEV(H$1:H$3)/SQRT(COUNT(H$1:H$3))</f>
-        <v>3.9903909838168966E-2</v>
+        <v>2.1967251752266336E-2</v>
       </c>
       <c r="J48">
         <f>STDEV(H$4:H$6)/SQRT(COUNT(H$4:H$6))</f>
-        <v>0.4998730592015192</v>
+        <v>0.14380117024004904</v>
       </c>
       <c r="K48">
         <f>STDEV(H$9:H$11)/SQRT(COUNT(H$9:H$11))</f>
-        <v>1.1366890449039642</v>
+        <v>2.9978342808046046</v>
       </c>
       <c r="L48">
         <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
-        <v>0.94764998627558839</v>
+        <v>2.4385643271491557</v>
       </c>
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.25">
@@ -2493,37 +2423,37 @@
       </c>
       <c r="J51">
         <f>AVERAGE(I$1:I$3)</f>
-        <v>5.7711096778619429E-2</v>
+        <v>4.7043281897724644E-2</v>
       </c>
       <c r="K51">
         <f>AVERAGE(I$4:I$6)</f>
-        <v>1.1171004640430429E-4</v>
+        <v>3.4991609077748002E-14</v>
       </c>
       <c r="L51">
         <f>AVERAGE(I$9:I$11)</f>
-        <v>1.8724526738434598E-9</v>
+        <v>2.9835877862400384E-9</v>
       </c>
       <c r="M51">
         <f>AVERAGE(I$13:I$16)</f>
-        <v>5.6875417269102668E-2</v>
+        <v>4.0530954529238379E-6</v>
       </c>
     </row>
     <row r="52" spans="9:16" x14ac:dyDescent="0.25">
       <c r="J52">
         <f>STDEV(I$1:I$3)/SQRT(COUNT(I$1:I$3))</f>
-        <v>5.7711043006897021E-2</v>
+        <v>4.7043281897702433E-2</v>
       </c>
       <c r="K52">
         <f>STDEV(I$4:I$6)/SQRT(COUNT(I$4:I$6))</f>
-        <v>1.1169307262540504E-4</v>
+        <v>6.3772773096146374E-15</v>
       </c>
       <c r="L52">
         <f>STDEV(I$9:I$11)/SQRT(COUNT(I$9:I$11))</f>
-        <v>1.8724249834283815E-9</v>
+        <v>2.983556279237191E-9</v>
       </c>
       <c r="M52">
         <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
-        <v>5.6875417269080464E-2</v>
+        <v>4.0529326997889823E-6</v>
       </c>
     </row>
     <row r="54" spans="9:16" x14ac:dyDescent="0.25">
@@ -2705,37 +2635,37 @@
       </c>
       <c r="N67">
         <f>AVERAGE(M$1:M$3)</f>
-        <v>0.996629973869819</v>
+        <v>0.99662997411815801</v>
       </c>
       <c r="O67">
         <f>AVERAGE(M$4:M$6)</f>
-        <v>0.99678503510959982</v>
+        <v>0.99678502774392774</v>
       </c>
       <c r="P67">
         <f>AVERAGE(M$9:M$11)</f>
-        <v>0.99445960073226625</v>
+        <v>0.9944596048642399</v>
       </c>
       <c r="Q67">
         <f>AVERAGE(M$13:M$16)</f>
-        <v>0.99613156400157077</v>
+        <v>0.99613211356786546</v>
       </c>
     </row>
     <row r="68" spans="13:20" x14ac:dyDescent="0.25">
       <c r="N68">
         <f>STDEV(M$1:M$3)/SQRT(COUNT(M$1:M$3))</f>
-        <v>4.9336881513329831E-4</v>
+        <v>4.9336913887755639E-4</v>
       </c>
       <c r="O68">
         <f>STDEV(M$4:M$6)/SQRT(COUNT(M$4:M$6))</f>
-        <v>3.4870120653301804E-4</v>
+        <v>3.486949347042988E-4</v>
       </c>
       <c r="P68">
         <f>STDEV(M$9:M$11)/SQRT(COUNT(M$9:M$11))</f>
-        <v>1.3128003017222126E-3</v>
+        <v>1.3127905162182648E-3</v>
       </c>
       <c r="Q68">
         <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
-        <v>1.68313394906313E-3</v>
+        <v>1.6834148194512729E-3</v>
       </c>
     </row>
     <row r="70" spans="13:20" x14ac:dyDescent="0.25">
@@ -2758,37 +2688,37 @@
       </c>
       <c r="O71">
         <f>AVERAGE(N$1:N$3)</f>
-        <v>0.99320520737618079</v>
+        <v>0.99199938412162059</v>
       </c>
       <c r="P71">
         <f>AVERAGE(N$4:N$6)</f>
-        <v>0.9768692652427774</v>
+        <v>0.97541479470508063</v>
       </c>
       <c r="Q71">
         <f>AVERAGE(N$7:N$12)</f>
-        <v>0.97646562260168146</v>
+        <v>0.97671749897086035</v>
       </c>
       <c r="R71">
         <f>AVERAGE(N$13:N$16)</f>
-        <v>0.99217205875359349</v>
+        <v>0.99258746444793977</v>
       </c>
     </row>
     <row r="72" spans="13:20" x14ac:dyDescent="0.25">
       <c r="O72">
         <f>STDEV(N$1:N$3)/SQRT(COUNT(N$1:N$3))</f>
-        <v>3.5671401184594262E-3</v>
+        <v>3.3666505227571966E-3</v>
       </c>
       <c r="P72">
         <f>STDEV(N$4:N$6)/SQRT(COUNT(N$4:N$6))</f>
-        <v>9.6914404714032783E-3</v>
+        <v>1.0654580102394942E-2</v>
       </c>
       <c r="Q72">
         <f>STDEV(N$9:N$11)/SQRT(COUNT(N$9:N$11))</f>
-        <v>1.1157447713336852E-2</v>
+        <v>1.1077469755827695E-2</v>
       </c>
       <c r="R72">
         <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
-        <v>2.7174487374415717E-3</v>
+        <v>2.5055085561655724E-3</v>
       </c>
     </row>
     <row r="74" spans="13:20" x14ac:dyDescent="0.25">
@@ -2811,37 +2741,37 @@
       </c>
       <c r="P75">
         <f>AVERAGE(O$1:O$3)</f>
-        <v>0.98952100355152439</v>
+        <v>0.99642630127703191</v>
       </c>
       <c r="Q75">
         <f>AVERAGE(O$4:O$6)</f>
-        <v>0.98808183356736645</v>
+        <v>0.98562172652789837</v>
       </c>
       <c r="R75">
         <f>AVERAGE(O$7:O$12)</f>
-        <v>0.98711557837146302</v>
+        <v>0.9844928740479385</v>
       </c>
       <c r="S75">
         <f>AVERAGE(O$13:O$16)</f>
-        <v>0.97501209567325531</v>
+        <v>0.96792446357023321</v>
       </c>
     </row>
     <row r="76" spans="13:20" x14ac:dyDescent="0.25">
       <c r="P76">
         <f>STDEV(O$1:O$3)/SQRT(COUNT(O$1:O$3))</f>
-        <v>6.2743065436297197E-3</v>
+        <v>7.903214212686805E-4</v>
       </c>
       <c r="Q76">
         <f>STDEV(O$4:O$6)/SQRT(COUNT(O$4:O$6))</f>
-        <v>5.9388891372863534E-3</v>
+        <v>9.0723300721945472E-3</v>
       </c>
       <c r="R76">
         <f>STDEV(O$9:O$11)/SQRT(COUNT(O$9:O$11))</f>
-        <v>3.5366108462667948E-3</v>
+        <v>3.4733597153074319E-3</v>
       </c>
       <c r="S76">
         <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
-        <v>1.2307008868033792E-2</v>
+        <v>9.1385974951318887E-3</v>
       </c>
     </row>
     <row r="78" spans="13:20" x14ac:dyDescent="0.25">
@@ -2864,37 +2794,37 @@
       </c>
       <c r="Q79">
         <f>AVERAGE(P$1:P$3)</f>
-        <v>8.2769960401192999E-2</v>
+        <v>8.2769960386286354E-2</v>
       </c>
       <c r="R79">
         <f>AVERAGE(P$4:P$6)</f>
-        <v>8.1747189231421533E-2</v>
+        <v>8.1747176174903999E-2</v>
       </c>
       <c r="S79">
         <f>AVERAGE(P$7:P$12)</f>
-        <v>0.1020035865843351</v>
+        <v>0.10199930527335742</v>
       </c>
       <c r="T79">
         <f>AVERAGE(P$13:P$16)</f>
-        <v>8.0500205067865718E-2</v>
+        <v>8.0488259007867796E-2</v>
       </c>
     </row>
     <row r="80" spans="13:20" x14ac:dyDescent="0.25">
       <c r="Q80">
         <f>STDEV(P$1:P$3)/SQRT(COUNT(P$1:P$3))</f>
-        <v>6.1728202192103884E-3</v>
+        <v>6.1728202303740097E-3</v>
       </c>
       <c r="R80">
         <f>STDEV(P$4:P$6)/SQRT(COUNT(P$4:P$6))</f>
-        <v>4.7620591820298364E-3</v>
+        <v>4.7620664425895532E-3</v>
       </c>
       <c r="S80">
         <f>STDEV(P$7:P$12)/SQRT(COUNT(P$7:P$12))</f>
-        <v>2.3059029941776794E-2</v>
+        <v>2.3060678578644904E-2</v>
       </c>
       <c r="T80">
         <f>STDEV(P$13:P$16)/SQRT(COUNT(P$13:P$16))</f>
-        <v>2.0136153727002573E-2</v>
+        <v>2.014243603928605E-2</v>
       </c>
     </row>
     <row r="82" spans="17:22" x14ac:dyDescent="0.25">
@@ -2917,37 +2847,37 @@
       </c>
       <c r="R83">
         <f>AVERAGE(Q$1:Q$3)</f>
-        <v>0.10959461994629464</v>
+        <v>0.12003209288401152</v>
       </c>
       <c r="S83">
         <f>AVERAGE(Q$4:Q$6)</f>
-        <v>0.21341357328280527</v>
+        <v>0.21343844914888963</v>
       </c>
       <c r="T83">
         <f>AVERAGE(Q$7:Q$12)</f>
-        <v>0.18093623769101944</v>
+        <v>0.1782439376864948</v>
       </c>
       <c r="U83">
         <f>AVERAGE(Q$13:Q$16)</f>
-        <v>0.12845495571043045</v>
+        <v>0.12579060832283959</v>
       </c>
     </row>
     <row r="84" spans="17:22" x14ac:dyDescent="0.25">
       <c r="R84">
         <f>STDEV(Q$1:Q$3)/SQRT(COUNT(Q$1:Q$3))</f>
-        <v>3.036014823577779E-2</v>
+        <v>2.9915209911607666E-2</v>
       </c>
       <c r="S84">
         <f>STDEV(Q$4:Q$6)/SQRT(COUNT(Q$4:Q$6))</f>
-        <v>4.5196413372371756E-2</v>
+        <v>4.3580024502883882E-2</v>
       </c>
       <c r="T84">
         <f>STDEV(Q$7:Q$12)/SQRT(COUNT(Q$7:Q$12))</f>
-        <v>5.4377126566252557E-2</v>
+        <v>5.5201478463506475E-2</v>
       </c>
       <c r="U84">
         <f>STDEV(Q$13:Q$16)/SQRT(COUNT(Q$13:Q$16))</f>
-        <v>2.7183622265906787E-2</v>
+        <v>2.5182325466262E-2</v>
       </c>
     </row>
     <row r="86" spans="17:22" x14ac:dyDescent="0.25">
@@ -2970,37 +2900,37 @@
       </c>
       <c r="S87">
         <f>AVERAGE(R$1:R$3)</f>
-        <v>0.14741060208624449</v>
+        <v>9.8876526846989221E-2</v>
       </c>
       <c r="T87">
         <f>AVERAGE(R$4:R$6)</f>
-        <v>0.1522140699475974</v>
+        <v>0.15989821775497828</v>
       </c>
       <c r="U87">
         <f>AVERAGE(R$7:R$12)</f>
-        <v>0.15636708683984385</v>
+        <v>0.17305949275824631</v>
       </c>
       <c r="V87">
         <f>AVERAGE(R$13:R$16)</f>
-        <v>0.25792063453863706</v>
+        <v>0.24531984414001679</v>
       </c>
     </row>
     <row r="88" spans="17:22" x14ac:dyDescent="0.25">
       <c r="S88">
         <f>STDEV(R$1:R$3)/SQRT(COUNT(R$1:R$3))</f>
-        <v>4.3333719769688396E-2</v>
+        <v>1.6225282641834871E-2</v>
       </c>
       <c r="T88">
         <f>STDEV(R$4:R$6)/SQRT(COUNT(R$4:R$6))</f>
-        <v>3.3710277588998395E-2</v>
+        <v>4.7075848425480959E-2</v>
       </c>
       <c r="U88">
         <f>STDEV(R$7:R$12)/SQRT(COUNT(R$7:R$12))</f>
-        <v>2.5752241582960484E-2</v>
+        <v>2.4291411337019984E-2</v>
       </c>
       <c r="V88">
         <f>STDEV(R$13:R$16)/SQRT(COUNT(R$13:R$16))</f>
-        <v>8.8331939902488374E-2</v>
+        <v>4.2744543922925191E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3054,4 +2984,533 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B38B132-172D-480B-8E20-0F35E7ADE26F}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>49.301247251052985</v>
+      </c>
+      <c r="C2">
+        <v>3.6597166972760207E-3</v>
+      </c>
+      <c r="D2">
+        <v>0.19023535438688108</v>
+      </c>
+      <c r="E2">
+        <v>20.57031599064171</v>
+      </c>
+      <c r="F2">
+        <v>2.2210033221700154E-14</v>
+      </c>
+      <c r="G2">
+        <v>0.14700895503484715</v>
+      </c>
+      <c r="H2">
+        <v>37.577113588733688</v>
+      </c>
+      <c r="I2">
+        <v>7.5917629324230532E-2</v>
+      </c>
+      <c r="J2">
+        <v>4.7043281897724644E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>49.618948169889904</v>
+      </c>
+      <c r="C3">
+        <v>1.2969578710698102E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.11098762168381754</v>
+      </c>
+      <c r="E3">
+        <v>19.737612962038288</v>
+      </c>
+      <c r="F3">
+        <v>2.8172663076369224E-7</v>
+      </c>
+      <c r="G3">
+        <v>0.51874426073426694</v>
+      </c>
+      <c r="H3">
+        <v>36.412781368255118</v>
+      </c>
+      <c r="I3">
+        <v>0.39118585551184881</v>
+      </c>
+      <c r="J3">
+        <v>3.4991609077748002E-14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>50.787001156938977</v>
+      </c>
+      <c r="C4">
+        <v>3.2467518098492486E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.14592261731789</v>
+      </c>
+      <c r="E4">
+        <v>17.201260815093182</v>
+      </c>
+      <c r="F4">
+        <v>3.5769692320523168E-4</v>
+      </c>
+      <c r="G4">
+        <v>1.5324904910997927</v>
+      </c>
+      <c r="H4">
+        <v>36.560668842267027</v>
+      </c>
+      <c r="I4">
+        <v>3.7994866553451856</v>
+      </c>
+      <c r="J4">
+        <v>2.9835877862400384E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>50.299346718483477</v>
+      </c>
+      <c r="C5">
+        <v>1.7436370403402304E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.12473897964381199</v>
+      </c>
+      <c r="E5">
+        <v>17.508245546550516</v>
+      </c>
+      <c r="F5">
+        <v>4.4129444733917032E-6</v>
+      </c>
+      <c r="G5">
+        <v>0.55341627633490109</v>
+      </c>
+      <c r="H5">
+        <v>36.549704624895277</v>
+      </c>
+      <c r="I5">
+        <v>2.6891949704917932</v>
+      </c>
+      <c r="J5">
+        <v>4.0530954529238379E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0.7455821156215362</v>
+      </c>
+      <c r="C8">
+        <v>1.3632467423976377E-4</v>
+      </c>
+      <c r="D8">
+        <v>3.4764251947037965E-2</v>
+      </c>
+      <c r="E8">
+        <v>5.508953379907469</v>
+      </c>
+      <c r="F8">
+        <v>4.8250618270174104E-18</v>
+      </c>
+      <c r="G8">
+        <v>3.7887236211488991E-2</v>
+      </c>
+      <c r="H8">
+        <v>6.3561831960480958E-2</v>
+      </c>
+      <c r="I8">
+        <v>2.1967251752266336E-2</v>
+      </c>
+      <c r="J8">
+        <v>4.7043281897702433E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.19684675716516564</v>
+      </c>
+      <c r="C9">
+        <v>2.8102841025300172E-3</v>
+      </c>
+      <c r="D9">
+        <v>0.10709949468666879</v>
+      </c>
+      <c r="E9">
+        <v>4.47375542154324</v>
+      </c>
+      <c r="F9">
+        <v>2.8172660276019622E-7</v>
+      </c>
+      <c r="G9">
+        <v>0.12579716058654763</v>
+      </c>
+      <c r="H9">
+        <v>0.49828508918370279</v>
+      </c>
+      <c r="I9">
+        <v>0.14380117024004904</v>
+      </c>
+      <c r="J9">
+        <v>6.3772773096146374E-15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.21296574375965627</v>
+      </c>
+      <c r="C10">
+        <v>1.8327582133541017E-2</v>
+      </c>
+      <c r="D10">
+        <v>7.0570066251987876E-2</v>
+      </c>
+      <c r="E10">
+        <v>2.5517362183417642</v>
+      </c>
+      <c r="F10">
+        <v>3.5769692317950405E-4</v>
+      </c>
+      <c r="G10">
+        <v>0.9089597995648262</v>
+      </c>
+      <c r="H10">
+        <v>0.49031258025953905</v>
+      </c>
+      <c r="I10">
+        <v>2.9978342808046046</v>
+      </c>
+      <c r="J10">
+        <v>2.983556279237191E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0.34670181381010645</v>
+      </c>
+      <c r="C11">
+        <v>9.1957167148318739E-3</v>
+      </c>
+      <c r="D11">
+        <v>7.3357716046404037E-2</v>
+      </c>
+      <c r="E11">
+        <v>3.9855119780421515</v>
+      </c>
+      <c r="F11">
+        <v>4.4127585456074152E-6</v>
+      </c>
+      <c r="G11">
+        <v>0.44401386483779698</v>
+      </c>
+      <c r="H11">
+        <v>0.39863100653210481</v>
+      </c>
+      <c r="I11">
+        <v>2.4385643271491557</v>
+      </c>
+      <c r="J11">
+        <v>4.0529326997889823E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(NOT(ISNUMBER(FIND("E",B2))),_xlfn.CONCAT(ROUND(B2,2), " ± ", ROUND(B8,2)),_xlfn.CONCAT(LEFT(B2,4),RIGHT(B2,4), " ± ",LEFT(B8,4),RIGHT(B8,4)))</f>
+        <v>49.3 ± 0.75</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ref="C13:J13" si="0">IF(NOT(ISNUMBER(FIND("E",C2))),_xlfn.CONCAT(ROUND(C2,2), " ± ", ROUND(C8,2)),_xlfn.CONCAT(LEFT(C2,4),RIGHT(C2,4), " ± ",LEFT(C8,4),RIGHT(C8,4)))</f>
+        <v>0 ± 0</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.19 ± 0.03</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>20.57 ± 5.51</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>2.22E-14 ± 4.82E-18</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.15 ± 0.04</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>37.58 ± 0.06</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.08 ± 0.02</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.05 ± 0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ref="B14:J16" si="1">IF(NOT(ISNUMBER(FIND("E",B3))),_xlfn.CONCAT(ROUND(B3,2), " ± ", ROUND(B9,2)),_xlfn.CONCAT(LEFT(B3,4),RIGHT(B3,4), " ± ",LEFT(B9,4),RIGHT(B9,4)))</f>
+        <v>49.62 ± 0.2</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.01 ± 0</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.11 ± 0.11</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>19.74 ± 4.47</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>2.81E-07 ± 2.81E-07</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.52 ± 0.13</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>36.41 ± 0.5</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.39 ± 0.14</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>3.49E-14 ± 6.37E-15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>50.79 ± 0.21</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.03 ± 0.02</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.15 ± 0.07</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>17.2 ± 2.55</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>0 ± 0</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>1.53 ± 0.91</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>36.56 ± 0.49</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>3.8 ± 3</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>2.98E-09 ± 2.98E-09</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>50.3 ± 0.35</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.02 ± 0.01</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.12 ± 0.07</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>17.51 ± 3.99</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>4.41E-06 ± 4.41E-06</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.55 ± 0.44</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>36.55 ± 0.4</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>2.69 ± 2.44</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>4.05E-06 ± 4.05E-06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Realized that FinalConfirmation and FinalConfirmation_T1Lin10s are identical
So I must have made some small error in the T1Lin10s that I can no longer track, but it doesn't really matter since the numbers are only different by small rounding errors
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3DC07C-C8F4-4FBB-BE1C-1E309A88C9CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B204F6E-CDCD-4E66-BB0E-BD9145FB79E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,6 +107,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,15 +457,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367D4110-0F05-4AA9-9660-0497C0778528}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:AB88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J52" sqref="J52:M52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>48.120613911731617</v>
       </c>
@@ -517,7 +521,7 @@
         <v>0.13102591930261462</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50.680396451715154</v>
       </c>
@@ -573,7 +577,7 @@
         <v>7.8981907325062134E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>49.102731389712162</v>
       </c>
@@ -629,7 +633,7 @@
         <v>8.6621753913290897E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50.012571778454578</v>
       </c>
@@ -685,7 +689,7 @@
         <v>0.25391303933089066</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>49.41571153061205</v>
       </c>
@@ -740,8 +744,41 @@
       <c r="R5">
         <v>0.11728586191248075</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T5" s="1">
+        <f>1/51</f>
+        <v>1.9607843137254902E-2</v>
+      </c>
+      <c r="U5">
+        <f>0.0001</f>
+        <v>1E-4</v>
+      </c>
+      <c r="V5">
+        <f>10^-8</f>
+        <v>1E-8</v>
+      </c>
+      <c r="W5" s="1">
+        <f>1/30-0.001</f>
+        <v>3.2333333333333332E-2</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>1E-3</v>
+      </c>
+      <c r="Z5" s="1">
+        <f>1/37.7</f>
+        <v>2.652519893899204E-2</v>
+      </c>
+      <c r="AA5">
+        <f>10^-8</f>
+        <v>1E-8</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>49.428561200603092</v>
       </c>
@@ -796,8 +833,38 @@
       <c r="R6">
         <v>0.10849575202156349</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T6" s="1">
+        <f>1/47</f>
+        <v>2.1276595744680851E-2</v>
+      </c>
+      <c r="U6">
+        <v>0.08</v>
+      </c>
+      <c r="V6">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1">
+        <f>1/10+0.001</f>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="X6">
+        <v>0.1</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="1">
+        <f>1/35.7</f>
+        <v>2.8011204481792715E-2</v>
+      </c>
+      <c r="AA6">
+        <v>10</v>
+      </c>
+      <c r="AB6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>49.134693742595658</v>
       </c>
@@ -853,7 +920,7 @@
         <v>9.123185443573037E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>48.970224341450667</v>
       </c>
@@ -909,7 +976,7 @@
         <v>0.21109361441809982</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50.361069671134324</v>
       </c>
@@ -965,7 +1032,7 @@
         <v>0.19874222923660653</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50.999999997994593</v>
       </c>
@@ -1021,7 +1088,7 @@
         <v>0.13578312841773169</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50.99993380168803</v>
       </c>
@@ -1077,7 +1144,7 @@
         <v>0.14608669072309458</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50.112410423624041</v>
       </c>
@@ -1133,7 +1200,7 @@
         <v>0.25541943931821498</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50.170242659167336</v>
       </c>
@@ -1189,7 +1256,7 @@
         <v>0.32512088803992523</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50.757253125081057</v>
       </c>
@@ -1245,7 +1312,7 @@
         <v>0.12637696756741412</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50.897187024056102</v>
       </c>
@@ -1301,7 +1368,7 @@
         <v>0.28282810134363656</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>49.372704065629407</v>
       </c>
@@ -1363,23 +1430,23 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="J17:Q32" si="0">_xlfn.IFS(ABS(1/B1-U$5)&lt;=0.001*(1/B1),"Lower",ABS(1/B1-U$6)&lt;=0.001*(1/B1),"Upper",TRUE,1)</f>
+        <f>_xlfn.IFS(ABS(B1-U$5)&lt;=0.001*(B1),"Lower",ABS(B1-U$6)&lt;=0.001*(B1),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(C1-V$5)&lt;=0.001*(C1),"Lower",ABS(C1-V$6)&lt;=0.001*(C1),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="L17">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J17:Q32" si="0">_xlfn.IFS(ABS(1/D1-W$5)&lt;=0.001*(1/D1),"Lower",ABS(1/D1-W$6)&lt;=0.001*(1/D1),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="M17">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(E1-X$5)&lt;=0.001*(E1),"Lower",ABS(E1-X$6)&lt;=0.001*(E1),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(F1-Y$5)&lt;=0.001*(F1),"Lower",ABS(F1-Y$6)&lt;=0.001*(F1),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="O17">
@@ -1387,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="P17">
-        <f t="shared" si="0"/>
+        <f>_xlfn.IFS(ABS(H1-AA$5)&lt;=0.001*(H1),"Lower",ABS(H1-AA$6)&lt;=0.001*(H1),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="Q17">
@@ -1413,23 +1480,23 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J18:K32" si="2">_xlfn.IFS(ABS(B2-U$5)&lt;=0.001*(B2),"Lower",ABS(B2-U$6)&lt;=0.001*(B2),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
       </c>
       <c r="M18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M18:N32" si="3">_xlfn.IFS(ABS(E2-X$5)&lt;=0.001*(E2),"Lower",ABS(E2-X$6)&lt;=0.001*(E2),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O18">
@@ -1437,11 +1504,11 @@
         <v>1</v>
       </c>
       <c r="P18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="P18:P32" si="4">_xlfn.IFS(ABS(H2-AA$5)&lt;=0.001*(H2),"Lower",ABS(H2-AA$6)&lt;=0.001*(H2),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q18:Q32" si="5">_xlfn.IFS(ABS(1/I2-AB$5)&lt;=0.001*(1/I2),"Lower",ABS(1/I2-AB$6)&lt;=0.001*(1/I2),"Upper",TRUE,1)</f>
         <v>1</v>
       </c>
     </row>
@@ -1470,11 +1537,11 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L19">
@@ -1482,11 +1549,11 @@
         <v>1</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O19">
@@ -1494,11 +1561,11 @@
         <v>1</v>
       </c>
       <c r="P19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1524,11 +1591,11 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L20">
@@ -1536,23 +1603,23 @@
         <v>1</v>
       </c>
       <c r="M20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
       </c>
       <c r="P20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="V20" t="e">
@@ -1566,11 +1633,11 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L21">
@@ -1578,11 +1645,11 @@
         <v>1</v>
       </c>
       <c r="M21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O21">
@@ -1590,11 +1657,11 @@
         <v>1</v>
       </c>
       <c r="P21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="V21" t="e">
@@ -1620,23 +1687,23 @@
         <v>1</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="2"/>
+        <v>Lower</v>
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O22">
@@ -1644,11 +1711,11 @@
         <v>1</v>
       </c>
       <c r="P22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="S22">
@@ -1689,11 +1756,11 @@
         <v>1</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L23">
@@ -1701,11 +1768,11 @@
         <v>1</v>
       </c>
       <c r="M23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O23">
@@ -1713,11 +1780,11 @@
         <v>1</v>
       </c>
       <c r="P23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1743,11 +1810,11 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L24">
@@ -1755,11 +1822,11 @@
         <v>1</v>
       </c>
       <c r="M24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O24">
@@ -1767,11 +1834,11 @@
         <v>1</v>
       </c>
       <c r="P24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1781,11 +1848,11 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L25">
@@ -1793,23 +1860,23 @@
         <v>1</v>
       </c>
       <c r="M25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1826,16 +1893,16 @@
       <c r="G26" t="s">
         <v>6</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L26">
@@ -1843,11 +1910,11 @@
         <v>1</v>
       </c>
       <c r="M26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O26">
@@ -1855,11 +1922,11 @@
         <v>1</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1883,16 +1950,16 @@
         <f>AVERAGE(C$13:C$16)</f>
         <v>0.12473897964381199</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v>Lower</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L27">
@@ -1900,11 +1967,11 @@
         <v>1</v>
       </c>
       <c r="M27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O27">
@@ -1912,11 +1979,11 @@
         <v>1</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1941,12 +2008,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="J28" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L28">
@@ -1954,11 +2021,11 @@
         <v>1</v>
       </c>
       <c r="M28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O28">
@@ -1966,11 +2033,11 @@
         <v>1</v>
       </c>
       <c r="P28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1980,11 +2047,11 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L29">
@@ -1992,11 +2059,11 @@
         <v>1</v>
       </c>
       <c r="M29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O29">
@@ -2004,11 +2071,11 @@
         <v>1</v>
       </c>
       <c r="P29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -2030,11 +2097,11 @@
         <v>1</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L30">
@@ -2042,11 +2109,11 @@
         <v>1</v>
       </c>
       <c r="M30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O30">
@@ -2054,11 +2121,11 @@
         <v>1</v>
       </c>
       <c r="P30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -2091,11 +2158,11 @@
         <v>1</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L31">
@@ -2103,11 +2170,11 @@
         <v>1</v>
       </c>
       <c r="M31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O31">
@@ -2115,11 +2182,11 @@
         <v>1</v>
       </c>
       <c r="P31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -2149,11 +2216,11 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L32">
@@ -2161,23 +2228,23 @@
         <v>1</v>
       </c>
       <c r="M32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="0"/>
+        <v>Upper</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="4"/>
+        <v>Upper</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -2991,7 +3058,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Did plot of T1L vs kPL
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928DC6D5-3836-42A8-BEFE-35C5E4833E7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD336D-77DF-4784-97C3-49AA3E64311E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4723,7 +4723,7 @@
   <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B11"/>
+      <selection activeCell="B22" sqref="B22:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7776,7 +7776,7 @@
         <v>79</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="C13:J13" si="0">IF(NOT(ISNUMBER(FIND("E",D2))),_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D8,2)),_xlfn.CONCAT(LEFT(D2,4),RIGHT(D2,4), " ± ",LEFT(D8,4),RIGHT(D8,4)))</f>
+        <f t="shared" ref="D13:J13" si="0">IF(NOT(ISNUMBER(FIND("E",D2))),_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D8,2)),_xlfn.CONCAT(LEFT(D2,4),RIGHT(D2,4), " ± ",LEFT(D8,4),RIGHT(D8,4)))</f>
         <v>0.19 ± 0.03</v>
       </c>
       <c r="E13" t="str">

</xml_diff>

<commit_message>
Saving output of previous commit
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECC3F76-38CB-407B-8FDB-BFE3BB567CF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C664FE1-B260-4B56-9B53-90C6C358BCAA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
@@ -5742,8 +5742,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:V88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
made some paired data changes
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D12CF7D-3EBE-4166-84AA-484E87357802}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BF9996-8B1F-4693-85F8-4B0911D35B63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="99">
   <si>
     <t>HK-2</t>
   </si>
@@ -330,6 +330,9 @@
   <si>
     <t>t Critical two-tail</t>
   </si>
+  <si>
+    <t>3.22533523075153</t>
+  </si>
 </sst>
 </file>
 
@@ -392,13 +395,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,7 +1057,7 @@
                     <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9089597995648262</c:v>
+                    <c:v>0.57387391232732432</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.44401386483779698</c:v>
@@ -1074,7 +1078,7 @@
                     <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9089597995648262</c:v>
+                    <c:v>0.57387391232732432</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.44401386483779698</c:v>
@@ -1129,7 +1133,7 @@
                   <c:v>0.51874426073426694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5324904910997927</c:v>
+                  <c:v>0.53726258101218571</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.55341627633490109</c:v>
@@ -5824,7 +5828,7 @@
   <dimension ref="A1:V88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6293,8 +6297,8 @@
       <c r="E9">
         <v>2.9250814687839763E-14</v>
       </c>
-      <c r="F9">
-        <v>3.2253352307515293</v>
+      <c r="F9" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="G9">
         <v>35.700000003988414</v>
@@ -7625,7 +7629,7 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E39">
         <f>STDEV(F5:F16)/SQRT(12)</f>
-        <v>0.28143020453412104</v>
+        <v>0.17158785109661681</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
@@ -7639,8 +7643,8 @@
         <v>0.51874426073426694</v>
       </c>
       <c r="I39">
-        <f>AVERAGE(F$9:F$11)</f>
-        <v>1.5324904910997927</v>
+        <f>AVERAGE(F$8:F$11)</f>
+        <v>0.53726258101218571</v>
       </c>
       <c r="J39">
         <f>AVERAGE(F$13:F$16)</f>
@@ -7658,7 +7662,7 @@
       </c>
       <c r="I40">
         <f>STDEV(F$9:F$11)/SQRT(COUNT(F$9:F$11))</f>
-        <v>0.9089597995648262</v>
+        <v>0.57387391232732432</v>
       </c>
       <c r="J40">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
@@ -8360,7 +8364,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8497,7 +8501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE390B71-28F5-46F9-948C-3E82AA0979A4}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -8635,8 +8639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFA7608-051E-4485-A7E9-B2F87390D8ED}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Made some changes to spreadsheet which included not excluding any UOK datapoints and making the summary slides to show Peder about paired data
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BF9996-8B1F-4693-85F8-4B0911D35B63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1D4C19-8676-42CD-8B62-329B590CD268}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="kpl paired" sheetId="4" r:id="rId2"/>
-    <sheet name="kmct4 paired" sheetId="5" r:id="rId3"/>
-    <sheet name="Paired Data" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Nothing Excluded" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
+    <sheet name="kpl paired" sheetId="4" r:id="rId4"/>
+    <sheet name="kmct4 paired" sheetId="5" r:id="rId5"/>
+    <sheet name="Paired Data" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="108">
   <si>
     <t>HK-2</t>
   </si>
@@ -331,7 +333,34 @@
     <t>t Critical two-tail</t>
   </si>
   <si>
-    <t>3.22533523075153</t>
+    <t>UOK</t>
+  </si>
+  <si>
+    <t>UOK+DIDS</t>
+  </si>
+  <si>
+    <t>UOK - (UOK + DIDS)</t>
+  </si>
+  <si>
+    <t>50.1 ± 0.36</t>
+  </si>
+  <si>
+    <t>0.04 ± 0.01</t>
+  </si>
+  <si>
+    <t>0.45 ± 0.32</t>
+  </si>
+  <si>
+    <t>19.25 ± 2.07</t>
+  </si>
+  <si>
+    <t>0.85 ± 0.51</t>
+  </si>
+  <si>
+    <t>36.74 ± 0.3</t>
+  </si>
+  <si>
+    <t>1.67E-07 ± 1.65E-07</t>
   </si>
 </sst>
 </file>
@@ -363,7 +392,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -391,11 +420,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -403,11 +447,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -638,7 +691,7 @@
                     <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.8327582133541017E-2</c:v>
+                    <c:v>1.2455011335729538E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>9.1957167148318739E-3</c:v>
@@ -659,7 +712,7 @@
                     <c:v>2.8102841025300172E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.8327582133541017E-2</c:v>
+                    <c:v>1.2455011335729538E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>9.1957167148318739E-3</c:v>
@@ -714,7 +767,7 @@
                   <c:v>1.2969578710698102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2467518098492486E-2</c:v>
+                  <c:v>3.6199003090424113E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.7436370403402304E-2</c:v>
@@ -1057,7 +1110,7 @@
                     <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.57387391232732432</c:v>
+                    <c:v>0.50916125182486183</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.44401386483779698</c:v>
@@ -1078,7 +1131,7 @@
                     <c:v>0.12579716058654763</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.57387391232732432</c:v>
+                    <c:v>0.50916125182486183</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.44401386483779698</c:v>
@@ -1133,7 +1186,7 @@
                   <c:v>0.51874426073426694</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53726258101218571</c:v>
+                  <c:v>0.84856895657055142</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.55341627633490109</c:v>
@@ -1333,36 +1386,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1495,7 +1518,7 @@
                     <c:v>0.19684675716516564</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.21296574375965627</c:v>
+                    <c:v>0.36038512706640941</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.34670181381010645</c:v>
@@ -1559,7 +1582,7 @@
                   <c:v>49.618948169889904</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.787001156938977</c:v>
+                  <c:v>50.096388663081221</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>50.299346718483477</c:v>
@@ -1570,6 +1593,291 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-509D-4131-A351-70158504402D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Paired Data'!$Q$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UOK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Paired Data'!$P$16:$P$23</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Paired Data'!$Q$16:$Q$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.1336378651585302E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8455085625926618E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.601888853618769E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9060525830266173E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6265635306323493E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23965150048870829</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11219420894660005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2253352307515293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D85E-4F2A-9FCF-EE8825B37CB9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Paired Data'!$R$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UOK+DIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Paired Data'!$P$16:$P$23</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Paired Data'!$R$16:$R$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.6403546782031753E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8323620306448935E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1560450572118007E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4712314332643145E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14710121465685502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1617351973594027E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15210747569666191</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8828390630124936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-D85E-4F2A-9FCF-EE8825B37CB9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Paired Data'!$S$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UOK - (UOK + DIDS)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Paired Data'!$P$16:$P$23</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kpl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>KMCT4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Paired Data'!$S$16:$S$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.6960239733821272E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3622723595281725E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4584379640696826E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4348211497623028E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.083557935053153E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20803414851511426</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.9913266750061863E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3424961677390357</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D85E-4F2A-9FCF-EE8825B37CB9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1924,7 +2232,7 @@
                     <c:v>0.49828508918370279</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.49031258025953905</c:v>
+                    <c:v>0.30295917840899245</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.39863100653210481</c:v>
@@ -1945,7 +2253,7 @@
                     <c:v>0.49828508918370279</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.49031258025953905</c:v>
+                    <c:v>0.30295917840899245</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>0.39863100653210481</c:v>
@@ -2000,7 +2308,7 @@
                   <c:v>36.412781368255118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.560668842267027</c:v>
+                  <c:v>36.73618734183853</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>36.549704624895277</c:v>
@@ -2364,7 +2672,7 @@
                     <c:v>4.47375542154324</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5517362183417642</c:v>
+                    <c:v>2.0724647254131807</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>3.9855119780421515</c:v>
@@ -2385,7 +2693,7 @@
                     <c:v>4.47375542154324</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5517362183417642</c:v>
+                    <c:v>2.0724647254131807</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>3.9855119780421515</c:v>
@@ -2440,7 +2748,7 @@
                   <c:v>19.737612962038288</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.201260815093182</c:v>
+                  <c:v>19.25031335600535</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17.508245546550516</c:v>
@@ -5418,16 +5726,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5827,8 +6135,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6297,8 +6605,8 @@
       <c r="E9">
         <v>2.9250814687839763E-14</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>98</v>
+      <c r="F9" s="4">
+        <v>3.2253352307515302</v>
       </c>
       <c r="G9">
         <v>35.700000003988414</v>
@@ -6830,8 +7138,8 @@
         <v>49.618948169889904</v>
       </c>
       <c r="D19">
-        <f>AVERAGE(A$9:A$11)</f>
-        <v>50.787001156938977</v>
+        <f>AVERAGE(A$7:A$12)</f>
+        <v>50.096388663081221</v>
       </c>
       <c r="E19">
         <f>AVERAGE(A$13:A$16)</f>
@@ -6884,8 +7192,8 @@
         <v>0.19684675716516564</v>
       </c>
       <c r="D20">
-        <f>STDEV(A$9:A$11)/SQRT(COUNT(A$9:A$11))</f>
-        <v>0.21296574375965627</v>
+        <f>STDEV(A$7:A$12)/SQRT(COUNT(A$7:A$12))</f>
+        <v>0.36038512706640941</v>
       </c>
       <c r="E20">
         <f>STDEV(A$13:A$16)/SQRT(COUNT(A$13:A$16))</f>
@@ -7049,8 +7357,8 @@
         <v>1.2969578710698102E-2</v>
       </c>
       <c r="E23">
-        <f>AVERAGE(B$9:B$11)</f>
-        <v>3.2467518098492486E-2</v>
+        <f>AVERAGE(B$7:B$12)</f>
+        <v>3.6199003090424113E-2</v>
       </c>
       <c r="F23">
         <f>AVERAGE(B$13:B$16)</f>
@@ -7103,8 +7411,8 @@
         <v>2.8102841025300172E-3</v>
       </c>
       <c r="E24">
-        <f>STDEV(B$9:B$11)/SQRT(COUNT(B$9:B$11))</f>
-        <v>1.8327582133541017E-2</v>
+        <f>STDEV(B$7:B$12)/SQRT(COUNT(B$7:B$12))</f>
+        <v>1.2455011335729538E-2</v>
       </c>
       <c r="F24">
         <f>STDEV(B$13:B$16)/SQRT(COUNT(B$13:B$16))</f>
@@ -7248,8 +7556,8 @@
         <v>0.11098762168381754</v>
       </c>
       <c r="F27">
-        <f>AVERAGE(C$9:C$11)</f>
-        <v>0.14592261731789</v>
+        <f>AVERAGE(C$7:C$12)</f>
+        <v>0.44574552826219332</v>
       </c>
       <c r="G27">
         <f>AVERAGE(C$13:C$16)</f>
@@ -7302,8 +7610,8 @@
         <v>0.10709949468666879</v>
       </c>
       <c r="F28">
-        <f>STDEV(C$9:C$11)/SQRT(COUNT(C$9:C$11))</f>
-        <v>7.0570066251987876E-2</v>
+        <f>STDEV(C$7:C$12)/SQRT(COUNT(C$7:C$12))</f>
+        <v>0.31845607936290327</v>
       </c>
       <c r="G28">
         <f>STDEV(C$13:C$16)/SQRT(COUNT(C$13:C$16))</f>
@@ -7451,8 +7759,8 @@
         <v>19.737612962038288</v>
       </c>
       <c r="G31">
-        <f>AVERAGE(D$9:D$11)</f>
-        <v>17.201260815093182</v>
+        <f>AVERAGE(D$7:D$12)</f>
+        <v>19.25031335600535</v>
       </c>
       <c r="H31">
         <f>AVERAGE(D$13:D$16)</f>
@@ -7509,8 +7817,8 @@
         <v>4.47375542154324</v>
       </c>
       <c r="G32">
-        <f>STDEV(D$9:D$11)/SQRT(COUNT(D$9:D$11))</f>
-        <v>2.5517362183417642</v>
+        <f>STDEV(D$7:D$12)/SQRT(COUNT(D$7:D$12))</f>
+        <v>2.0724647254131807</v>
       </c>
       <c r="H32">
         <f>STDEV(D$13:D$16)/SQRT(COUNT(D$13:D$16))</f>
@@ -7586,8 +7894,8 @@
         <v>2.8172663076369224E-7</v>
       </c>
       <c r="H35">
-        <f>AVERAGE(E$9:E$11)</f>
-        <v>3.5769692320523168E-4</v>
+        <f>AVERAGE(E$7:E$12)</f>
+        <v>5.9381575747716945E-4</v>
       </c>
       <c r="I35">
         <f>AVERAGE(E$13:E$16)</f>
@@ -7604,8 +7912,8 @@
         <v>2.8172660276019622E-7</v>
       </c>
       <c r="H36">
-        <f>STDEV(E$9:E$11)/SQRT(COUNT(E$9:E$11))</f>
-        <v>3.5769692317950405E-4</v>
+        <f>STDEV(E$7:E$12)/SQRT(COUNT(E$7:E$12))</f>
+        <v>4.1772971629201147E-4</v>
       </c>
       <c r="I36">
         <f>STDEV(E$13:E$16)/SQRT(COUNT(E$13:E$16))</f>
@@ -7629,7 +7937,7 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E39">
         <f>STDEV(F5:F16)/SQRT(12)</f>
-        <v>0.17158785109661681</v>
+        <v>0.28143020453412115</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
@@ -7643,8 +7951,8 @@
         <v>0.51874426073426694</v>
       </c>
       <c r="I39">
-        <f>AVERAGE(F$8:F$11)</f>
-        <v>0.53726258101218571</v>
+        <f>AVERAGE(F$7:F$12)</f>
+        <v>0.84856895657055142</v>
       </c>
       <c r="J39">
         <f>AVERAGE(F$13:F$16)</f>
@@ -7661,8 +7969,8 @@
         <v>0.12579716058654763</v>
       </c>
       <c r="I40">
-        <f>STDEV(F$9:F$11)/SQRT(COUNT(F$9:F$11))</f>
-        <v>0.57387391232732432</v>
+        <f>STDEV(F$7:F$12)/SQRT(COUNT(F$7:F$12))</f>
+        <v>0.50916125182486183</v>
       </c>
       <c r="J40">
         <f>STDEV(F$13:F$16)/SQRT(COUNT(F$13:F$16))</f>
@@ -7696,8 +8004,8 @@
         <v>36.412781368255118</v>
       </c>
       <c r="J43">
-        <f>AVERAGE(G$9:G$11)</f>
-        <v>36.560668842267027</v>
+        <f>AVERAGE(G$7:G$12)</f>
+        <v>36.73618734183853</v>
       </c>
       <c r="K43">
         <f>AVERAGE(G$13:G$16)</f>
@@ -7714,8 +8022,8 @@
         <v>0.49828508918370279</v>
       </c>
       <c r="J44">
-        <f>STDEV(G$9:G$11)/SQRT(COUNT(G$9:G$11))</f>
-        <v>0.49031258025953905</v>
+        <f>STDEV(G$7:G$12)/SQRT(COUNT(G$7:G$12))</f>
+        <v>0.30295917840899245</v>
       </c>
       <c r="K44">
         <f>STDEV(G$13:G$16)/SQRT(COUNT(G$13:G$16))</f>
@@ -7749,8 +8057,8 @@
         <v>0.39118585551184881</v>
       </c>
       <c r="K47">
-        <f>AVERAGE(H$9:H$11)</f>
-        <v>3.7994866553451856</v>
+        <f>AVERAGE(H$7:H$12)</f>
+        <v>2.073731176478951</v>
       </c>
       <c r="L47">
         <f>AVERAGE(H$13:H$16)</f>
@@ -7767,8 +8075,8 @@
         <v>0.14380117024004904</v>
       </c>
       <c r="K48">
-        <f>STDEV(H$9:H$11)/SQRT(COUNT(H$9:H$11))</f>
-        <v>2.9978342808046046</v>
+        <f>STDEV(H$7:H$12)/SQRT(COUNT(H$7:H$12))</f>
+        <v>1.5481644036824562</v>
       </c>
       <c r="L48">
         <f>STDEV(H$13:H$16)/SQRT(COUNT(H$13:H$16))</f>
@@ -7802,8 +8110,8 @@
         <v>3.4991609077748002E-14</v>
       </c>
       <c r="L51">
-        <f>AVERAGE(I$9:I$11)</f>
-        <v>2.9835877862400384E-9</v>
+        <f>AVERAGE(I$7:I$12)</f>
+        <v>1.6718958224935493E-7</v>
       </c>
       <c r="M51">
         <f>AVERAGE(I$13:I$16)</f>
@@ -7820,8 +8128,8 @@
         <v>6.3772773096146374E-15</v>
       </c>
       <c r="L52">
-        <f>STDEV(I$9:I$11)/SQRT(COUNT(I$9:I$11))</f>
-        <v>2.983556279237191E-9</v>
+        <f>STDEV(I$7:I$12)/SQRT(COUNT(I$7:I$12))</f>
+        <v>1.6540587478552495E-7</v>
       </c>
       <c r="M52">
         <f>STDEV(I$13:I$16)/SQRT(COUNT(I$13:I$16))</f>
@@ -7855,8 +8163,8 @@
         <v>4.5811578254944498</v>
       </c>
       <c r="M55">
-        <f>AVERAGE(J$9:J$11)</f>
-        <v>3.6056343285878296</v>
+        <f>AVERAGE(J$7:J$12)</f>
+        <v>3.4256186710021974</v>
       </c>
       <c r="N55">
         <f>AVERAGE(J$13:J$16)</f>
@@ -7873,8 +8181,8 @@
         <v>0.74102585341338212</v>
       </c>
       <c r="M56">
-        <f>STDEV(J$9:J$11)/SQRT(COUNT(J$9:J$11))</f>
-        <v>0.42588055523052337</v>
+        <f>STDEV(J$7:J$12)/SQRT(COUNT(J$7:J$12))</f>
+        <v>0.51601445159187342</v>
       </c>
       <c r="N56">
         <f>STDEV(J$13:J$16)/SQRT(COUNT(J$13:J$16))</f>
@@ -7908,8 +8216,8 @@
         <v>14.884031830230191</v>
       </c>
       <c r="N59">
-        <f>AVERAGE(K$9:K$11)</f>
-        <v>16.201058340567712</v>
+        <f>AVERAGE(K$7:K$12)</f>
+        <v>17.702043971074474</v>
       </c>
       <c r="O59">
         <f>AVERAGE(K$13:K$16)</f>
@@ -7926,8 +8234,8 @@
         <v>2.7073905114872208</v>
       </c>
       <c r="N60">
-        <f>STDEV(K$9:K$11)/SQRT(COUNT(K$9:K$11))</f>
-        <v>3.3207187374732552</v>
+        <f>STDEV(K$7:K$12)/SQRT(COUNT(K$7:K$12))</f>
+        <v>1.7513483951030933</v>
       </c>
       <c r="O60">
         <f>STDEV(K$13:K$16)/SQRT(COUNT(K$13:K$16))</f>
@@ -7961,8 +8269,8 @@
         <v>307023757.75154978</v>
       </c>
       <c r="O63">
-        <f>AVERAGE(L$9:L$11)</f>
-        <v>444284473.67489415</v>
+        <f>AVERAGE(L$7:L$12)</f>
+        <v>537300475.99648142</v>
       </c>
       <c r="P63">
         <f>AVERAGE(L$13:L$16)</f>
@@ -7979,8 +8287,8 @@
         <v>161012746.78001404</v>
       </c>
       <c r="O64">
-        <f>STDEV(L$9:L$11)/SQRT(COUNT(L$9:L$11))</f>
-        <v>380817343.30973661</v>
+        <f>STDEV(L$7:L$12)/SQRT(COUNT(L$7:L$12))</f>
+        <v>234388492.25677821</v>
       </c>
       <c r="P64">
         <f>STDEV(L$13:L$16)/SQRT(COUNT(L$13:L$16))</f>
@@ -8014,8 +8322,8 @@
         <v>0.99678502774392774</v>
       </c>
       <c r="P67">
-        <f>AVERAGE(M$9:M$11)</f>
-        <v>0.9944596048642399</v>
+        <f>AVERAGE(M$7:M$12)</f>
+        <v>0.99341790526897988</v>
       </c>
       <c r="Q67">
         <f>AVERAGE(M$13:M$16)</f>
@@ -8032,8 +8340,8 @@
         <v>3.486949347042988E-4</v>
       </c>
       <c r="P68">
-        <f>STDEV(M$9:M$11)/SQRT(COUNT(M$9:M$11))</f>
-        <v>1.3127905162182648E-3</v>
+        <f>STDEV(M$7:M$12)/SQRT(COUNT(M$7:M$12))</f>
+        <v>2.9228090901447677E-3</v>
       </c>
       <c r="Q68">
         <f>STDEV(M$13:M$16)/SQRT(COUNT(M$13:M$16))</f>
@@ -8085,8 +8393,8 @@
         <v>1.0654580102394942E-2</v>
       </c>
       <c r="Q72">
-        <f>STDEV(N$9:N$11)/SQRT(COUNT(N$9:N$11))</f>
-        <v>1.1077469755827695E-2</v>
+        <f>STDEV(N$7:N$12)/SQRT(COUNT(N$7:N$12))</f>
+        <v>1.2661181912125088E-2</v>
       </c>
       <c r="R72">
         <f>STDEV(N$13:N$16)/SQRT(COUNT(N$13:N$16))</f>
@@ -8138,8 +8446,8 @@
         <v>9.0723300721945472E-3</v>
       </c>
       <c r="R76">
-        <f>STDEV(O$9:O$11)/SQRT(COUNT(O$9:O$11))</f>
-        <v>3.4733597153074319E-3</v>
+        <f>STDEV(O$7:O$12)/SQRT(COUNT(O$7:O$12))</f>
+        <v>4.5865293474133487E-3</v>
       </c>
       <c r="S76">
         <f>STDEV(O$13:O$16)/SQRT(COUNT(O$13:O$16))</f>
@@ -8360,7 +8668,827 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825B98BF-6048-4BE4-8343-B7D5D51D380B}">
+  <dimension ref="A1:S16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:S10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>49.301247251052985</v>
+      </c>
+      <c r="C2">
+        <v>3.6597166972760207E-3</v>
+      </c>
+      <c r="D2">
+        <v>0.19023535438688108</v>
+      </c>
+      <c r="E2">
+        <v>20.57031599064171</v>
+      </c>
+      <c r="F2">
+        <v>2.2210033221700154E-14</v>
+      </c>
+      <c r="G2">
+        <v>0.14700895503484715</v>
+      </c>
+      <c r="H2">
+        <v>37.577113588733688</v>
+      </c>
+      <c r="I2">
+        <v>7.5917629324230532E-2</v>
+      </c>
+      <c r="J2">
+        <v>4.7043281897724644E-2</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>49.618948169889904</v>
+      </c>
+      <c r="C3">
+        <v>1.2969578710698102E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.11098762168381754</v>
+      </c>
+      <c r="E3">
+        <v>19.737612962038288</v>
+      </c>
+      <c r="F3">
+        <v>2.8172663076369224E-7</v>
+      </c>
+      <c r="G3">
+        <v>0.51874426073426694</v>
+      </c>
+      <c r="H3">
+        <v>36.412781368255118</v>
+      </c>
+      <c r="I3">
+        <v>0.39118585551184881</v>
+      </c>
+      <c r="J3">
+        <v>3.4991609077748002E-14</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>50.096388663081221</v>
+      </c>
+      <c r="C4">
+        <v>3.6199003090424113E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.44574552826219332</v>
+      </c>
+      <c r="E4">
+        <v>19.25031335600535</v>
+      </c>
+      <c r="F4">
+        <v>5.9381575747716945E-4</v>
+      </c>
+      <c r="G4">
+        <v>0.84856895657055142</v>
+      </c>
+      <c r="H4">
+        <v>36.73618734183853</v>
+      </c>
+      <c r="I4">
+        <v>2.073731176478951</v>
+      </c>
+      <c r="J4">
+        <v>1.6718958224935493E-7</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>50.299346718483477</v>
+      </c>
+      <c r="C5">
+        <v>1.7436370403402304E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.12473897964381199</v>
+      </c>
+      <c r="E5">
+        <v>17.508245546550516</v>
+      </c>
+      <c r="F5">
+        <v>4.4129444733917032E-6</v>
+      </c>
+      <c r="G5">
+        <v>0.55341627633490109</v>
+      </c>
+      <c r="H5">
+        <v>36.549704624895277</v>
+      </c>
+      <c r="I5">
+        <v>2.6891949704917932</v>
+      </c>
+      <c r="J5">
+        <v>4.0530954529238379E-6</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0.7455821156215362</v>
+      </c>
+      <c r="C8">
+        <v>1.3632467423976377E-4</v>
+      </c>
+      <c r="D8">
+        <v>3.4764251947037965E-2</v>
+      </c>
+      <c r="E8">
+        <v>5.508953379907469</v>
+      </c>
+      <c r="F8">
+        <v>4.8250618270174104E-18</v>
+      </c>
+      <c r="G8">
+        <v>3.7887236211488991E-2</v>
+      </c>
+      <c r="H8">
+        <v>6.3561831960480958E-2</v>
+      </c>
+      <c r="I8">
+        <v>2.1967251752266336E-2</v>
+      </c>
+      <c r="J8">
+        <v>4.7043281897702433E-2</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.19684675716516564</v>
+      </c>
+      <c r="C9">
+        <v>2.8102841025300172E-3</v>
+      </c>
+      <c r="D9">
+        <v>0.10709949468666879</v>
+      </c>
+      <c r="E9">
+        <v>4.47375542154324</v>
+      </c>
+      <c r="F9">
+        <v>2.8172660276019622E-7</v>
+      </c>
+      <c r="G9">
+        <v>0.12579716058654763</v>
+      </c>
+      <c r="H9">
+        <v>0.49828508918370279</v>
+      </c>
+      <c r="I9">
+        <v>0.14380117024004904</v>
+      </c>
+      <c r="J9">
+        <v>6.3772773096146374E-15</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.36038512706640941</v>
+      </c>
+      <c r="C10">
+        <v>1.2455011335729538E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.31845607936290327</v>
+      </c>
+      <c r="E10">
+        <v>2.0724647254131807</v>
+      </c>
+      <c r="F10">
+        <v>4.1772971629201147E-4</v>
+      </c>
+      <c r="G10">
+        <v>0.50916125182486183</v>
+      </c>
+      <c r="H10">
+        <v>0.30295917840899245</v>
+      </c>
+      <c r="I10">
+        <v>1.5481644036824562</v>
+      </c>
+      <c r="J10">
+        <v>1.6540587478552495E-7</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0.34670181381010645</v>
+      </c>
+      <c r="C11">
+        <v>9.1957167148318739E-3</v>
+      </c>
+      <c r="D11">
+        <v>7.3357716046404037E-2</v>
+      </c>
+      <c r="E11">
+        <v>3.9855119780421515</v>
+      </c>
+      <c r="F11">
+        <v>4.4127585456074152E-6</v>
+      </c>
+      <c r="G11">
+        <v>0.44401386483779698</v>
+      </c>
+      <c r="H11">
+        <v>0.39863100653210481</v>
+      </c>
+      <c r="I11">
+        <v>2.4385643271491557</v>
+      </c>
+      <c r="J11">
+        <v>4.0529326997889823E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(NOT(ISNUMBER(FIND("E",B2))),_xlfn.CONCAT(ROUND(B2,2), " ± ", ROUND(B8,2)),_xlfn.CONCAT(LEFT(B2,4),RIGHT(B2,4), " ± ",LEFT(B8,4),RIGHT(B8,4)))</f>
+        <v>49.3 ± 0.75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:J13" si="0">IF(NOT(ISNUMBER(FIND("E",D2))),_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D8,2)),_xlfn.CONCAT(LEFT(D2,4),RIGHT(D2,4), " ± ",LEFT(D8,4),RIGHT(D8,4)))</f>
+        <v>0.19 ± 0.03</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>20.57 ± 5.51</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>2.22E-14 ± 4.82E-18</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.15 ± 0.04</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>37.58 ± 0.06</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.08 ± 0.02</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.05 ± 0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ref="B14:J16" si="1">IF(NOT(ISNUMBER(FIND("E",B3))),_xlfn.CONCAT(ROUND(B3,2), " ± ", ROUND(B9,2)),_xlfn.CONCAT(LEFT(B3,4),RIGHT(B3,4), " ± ",LEFT(B9,4),RIGHT(B9,4)))</f>
+        <v>49.62 ± 0.2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.11 ± 0.11</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>19.74 ± 4.47</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>2.81E-07 ± 2.81E-07</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.52 ± 0.13</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>36.41 ± 0.5</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>0.39 ± 0.14</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>3.49E-14 ± 6.37E-15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>50.1 ± 0.36</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.04 ± 0.01</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.45 ± 0.32</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>19.25 ± 2.07</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>0.85 ± 0.51</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>36.74 ± 0.3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>1.67E-07 ± 1.65E-07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>50.3 ± 0.35</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.02 ± 0.01</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.12 ± 0.07</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>17.51 ± 3.99</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>4.41E-06 ± 4.41E-06</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>0.55 ± 0.44</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>36.55 ± 0.4</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>2.69 ± 2.44</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>4.05E-06 ± 4.05E-06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442BFD65-9632-480E-B7DB-71471588CBEA}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>3.4795161265732725E-3</v>
+      </c>
+      <c r="C2">
+        <v>8.2261049334318315E-3</v>
+      </c>
+      <c r="D2">
+        <v>1.1336378651585302E-2</v>
+      </c>
+      <c r="E2">
+        <v>8.6403546782031753E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>3.9270147990883662E-3</v>
+      </c>
+      <c r="C3">
+        <v>1.7952384844695909E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.8455085625926618E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.8323620306448935E-3</v>
+      </c>
+      <c r="K3">
+        <v>3.4795161265732725E-3</v>
+      </c>
+      <c r="L3">
+        <v>3.9270147990883662E-3</v>
+      </c>
+      <c r="M3">
+        <v>3.5726191661664243E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>3.5726191661664243E-3</v>
+      </c>
+      <c r="C4">
+        <v>1.2730246353966567E-2</v>
+      </c>
+      <c r="D4">
+        <v>6.9060525830266173E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.1560450572118007E-2</v>
+      </c>
+      <c r="K4">
+        <v>8.2261049334318315E-3</v>
+      </c>
+      <c r="L4">
+        <v>1.7952384844695909E-2</v>
+      </c>
+      <c r="M4">
+        <v>1.2730246353966567E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1.2323139929023586E-2</v>
+      </c>
+      <c r="E5">
+        <v>4.4712314332643145E-2</v>
+      </c>
+      <c r="K5">
+        <v>1.1336378651585302E-2</v>
+      </c>
+      <c r="L5">
+        <v>2.8455085625926618E-2</v>
+      </c>
+      <c r="M5">
+        <v>6.9060525830266173E-2</v>
+      </c>
+      <c r="N5">
+        <v>1.2323139929023586E-2</v>
+      </c>
+      <c r="O5">
+        <v>1.601888853618769E-2</v>
+      </c>
+      <c r="P5">
+        <v>7.9999999969555299E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>1.601888853618769E-2</v>
+      </c>
+      <c r="K6">
+        <v>8.6403546782031753E-3</v>
+      </c>
+      <c r="L6">
+        <v>4.8323620306448935E-3</v>
+      </c>
+      <c r="M6">
+        <v>1.1560450572118007E-2</v>
+      </c>
+      <c r="N6">
+        <v>4.4712314332643145E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>7.9999999969555299E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00219993-CFD6-4B07-9FE3-775345900DDF}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8497,8 +9625,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE390B71-28F5-46F9-948C-3E82AA0979A4}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8635,15 +9764,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFA7608-051E-4485-A7E9-B2F87390D8ED}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15:S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="19" max="19" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -9233,6 +10366,16 @@
         <f t="shared" si="0"/>
         <v>0.98836560550491726</v>
       </c>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -9269,8 +10412,21 @@
         <f t="shared" si="0"/>
         <v>2.4348211497623028E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>1.1336378651585302E-2</v>
+      </c>
+      <c r="R16" s="5">
+        <v>8.6403546782031753E-3</v>
+      </c>
+      <c r="S16" s="5">
+        <f>Q16-R16</f>
+        <v>2.6960239733821272E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -9305,8 +10461,21 @@
         <f t="shared" si="0"/>
         <v>-8.0643576878476619E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>2.8455085625926618E-2</v>
+      </c>
+      <c r="R17" s="5">
+        <v>4.8323620306448935E-3</v>
+      </c>
+      <c r="S17" s="5">
+        <f t="shared" ref="S17:S23" si="2">Q17-R17</f>
+        <v>2.3622723595281725E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -9341,8 +10510,21 @@
         <f t="shared" si="0"/>
         <v>3.4991351471543304</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>1.601888853618769E-2</v>
+      </c>
+      <c r="R18" s="5">
+        <v>1.1560450572118007E-2</v>
+      </c>
+      <c r="S18" s="5">
+        <f t="shared" si="2"/>
+        <v>4.4584379640696826E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -9377,8 +10559,21 @@
         <f t="shared" si="0"/>
         <v>7.046354195336632E-15</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>6.9060525830266173E-2</v>
+      </c>
+      <c r="R19" s="5">
+        <v>4.4712314332643145E-2</v>
+      </c>
+      <c r="S19" s="5">
+        <f t="shared" si="2"/>
+        <v>2.4348211497623028E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -9413,8 +10608,21 @@
         <f t="shared" si="0"/>
         <v>1.3424961677390357</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>7.6265635306323493E-2</v>
+      </c>
+      <c r="R20" s="5">
+        <v>0.14710121465685502</v>
+      </c>
+      <c r="S20" s="5">
+        <f t="shared" si="2"/>
+        <v>-7.083557935053153E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -9449,8 +10657,21 @@
         <f t="shared" si="0"/>
         <v>3.9600607237844088E-9</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>0.23965150048870829</v>
+      </c>
+      <c r="R21" s="5">
+        <v>3.1617351973594027E-2</v>
+      </c>
+      <c r="S21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.20803414851511426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -9485,8 +10706,21 @@
         <f t="shared" si="0"/>
         <v>-0.24934534038626666</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>0.11219420894660005</v>
+      </c>
+      <c r="R22" s="5">
+        <v>0.15210747569666191</v>
+      </c>
+      <c r="S22" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.9913266750061863E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -9521,8 +10755,21 @@
         <f t="shared" si="0"/>
         <v>8.4625056563750924E-9</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>3.2253352307515293</v>
+      </c>
+      <c r="R23" s="5">
+        <v>1.8828390630124936</v>
+      </c>
+      <c r="S23" s="5">
+        <f t="shared" si="2"/>
+        <v>1.3424961677390357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -9539,7 +10786,7 @@
         <v>49.372704065629407</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -9556,7 +10803,7 @@
         <v>4.4712314332643145E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -9573,7 +10820,7 @@
         <v>0.33865466146936779</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -9590,7 +10837,7 @@
         <v>9.9724964073016142</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -9607,7 +10854,7 @@
         <v>2.2204460492503131E-14</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -9624,7 +10871,7 @@
         <v>1.8828390630124936</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -9641,7 +10888,7 @@
         <v>35.700000000028353</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -9658,7 +10905,7 @@
         <v>9.9999999999999787</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -9677,6 +10924,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q2">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -9688,7 +10971,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2">
+  <conditionalFormatting sqref="R3">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -9700,7 +10983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2">
+  <conditionalFormatting sqref="S3">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -9712,7 +10995,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3">
+  <conditionalFormatting sqref="Q5">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -9724,7 +11007,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3">
+  <conditionalFormatting sqref="R5">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -9736,7 +11019,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3">
+  <conditionalFormatting sqref="S5">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -9748,7 +11031,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5">
+  <conditionalFormatting sqref="Q6">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -9760,7 +11043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5">
+  <conditionalFormatting sqref="R6">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -9772,7 +11055,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S5">
+  <conditionalFormatting sqref="S6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -9784,7 +11067,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q6">
+  <conditionalFormatting sqref="Q8">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -9796,7 +11079,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6">
+  <conditionalFormatting sqref="R8">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -9808,7 +11091,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S6">
+  <conditionalFormatting sqref="S8">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -9820,7 +11103,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q8">
+  <conditionalFormatting sqref="Q9">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -9832,7 +11115,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R8">
+  <conditionalFormatting sqref="R9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -9844,7 +11127,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S8">
+  <conditionalFormatting sqref="S9">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -9856,7 +11139,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q9">
+  <conditionalFormatting sqref="Q11">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -9868,7 +11151,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R9">
+  <conditionalFormatting sqref="R11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -9880,7 +11163,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
+  <conditionalFormatting sqref="S11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -9892,7 +11175,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q11">
+  <conditionalFormatting sqref="Q12">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -9904,7 +11187,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
+  <conditionalFormatting sqref="R12">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -9916,7 +11199,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
+  <conditionalFormatting sqref="S12">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -9928,53 +11211,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q12">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R12">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="S16:S23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B38B132-172D-480B-8E20-0F35E7ADE26F}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10014,16 +11267,17 @@
       <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N1" s="5"/>
+      <c r="O1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="P1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10058,19 +11312,19 @@
       <c r="J2">
         <v>4.7043281897724644E-2</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -10105,19 +11359,19 @@
       <c r="J3">
         <v>3.4991609077748002E-14</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -10152,19 +11406,19 @@
       <c r="J4">
         <v>2.9835877862400384E-9</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -10199,36 +11453,36 @@
       <c r="J5">
         <v>4.0530954529238379E-6</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="N6" t="s">
+      <c r="N6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -10260,19 +11514,19 @@
       <c r="J7" t="s">
         <v>13</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -10307,19 +11561,19 @@
       <c r="J8">
         <v>4.7043281897702433E-2</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -10354,19 +11608,19 @@
       <c r="J9">
         <v>6.3772773096146374E-15</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -10401,19 +11655,19 @@
       <c r="J10">
         <v>2.983556279237191E-9</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="5" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tried running loops, but failed because of some NaN error in Pyr_starting_out that I'm trying to fix
</commit_message>
<xml_diff>
--- a/Lacex_summary_FinalConfirmation.xlsx
+++ b/Lacex_summary_FinalConfirmation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851163AA-BD2B-4358-BBE2-532186E40C6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A6524A-50F9-40D9-9144-09EAA8E7ADBF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="12" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
+    <workbookView xWindow="-23148" yWindow="0" windowWidth="23256" windowHeight="12576" xr2:uid="{C3D14B4C-3BE8-4F56-A36A-8E13C19772D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5716,16 +5716,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5752,16 +5752,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>451485</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>146685</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6197,8 +6197,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10469,7 +10469,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>